<commit_message>
Updated simulation builder & added sensor analysis excel
</commit_message>
<xml_diff>
--- a/results/sensoranalysis.xlsx
+++ b/results/sensoranalysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="21075" windowHeight="11055"/>
+    <workbookView xWindow="360" yWindow="180" windowWidth="21075" windowHeight="10995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="51">
   <si>
     <t>Group</t>
   </si>
@@ -167,12 +167,15 @@
   <si>
     <t>x</t>
   </si>
+  <si>
+    <t>NULL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,8 +205,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,8 +244,18 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -405,12 +432,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -444,9 +488,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -464,8 +505,15 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="3"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -520,8 +568,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -529,10 +577,7 @@
           <c:tx>
             <c:v>16 TIM groups, 5 slots</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$H$88:$H$92</c:f>
               <c:numCache>
@@ -555,8 +600,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>(Sheet1!$J$15,Sheet1!$J$45,Sheet1!$J$63,Sheet1!$J$74,Sheet1!$J$85)</c:f>
               <c:numCache>
@@ -579,19 +624,16 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>12 TIM groups, 2 slots</c:v>
+            <c:v>16 TIM groups, 2 slots</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$H$88:$H$92</c:f>
               <c:numCache>
@@ -614,43 +656,40 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>(Sheet1!$I$14,Sheet1!$I$44,Sheet1!$I$62,Sheet1!$I$73,Sheet1!$I$84)</c:f>
+              <c:f>(Sheet1!$J$14,Sheet1!$J$44,Sheet1!$J$62,Sheet1!$J$73,Sheet1!$J$84)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>59</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>119</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>149</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>149</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>149</c:v>
+                  <c:v>214</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>8 TIM groups, 10 slots</c:v>
+            <c:v>16 TIM groups, 10 slots</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$H$88:$H$92</c:f>
               <c:numCache>
@@ -673,32 +712,88 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>(Sheet1!$H$16,Sheet1!$H$46,Sheet1!$H$64,Sheet1!$H$75,Sheet1!$H$86)</c:f>
+              <c:f>(Sheet1!$J$16,Sheet1!$J$46,Sheet1!$J$64,Sheet1!$J$75,Sheet1!$J$86)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>44</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>64</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>16 TIM groups, 1 slot</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$88:$H$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Sheet1!$J$13,Sheet1!$J$43,Sheet1!$J$61,Sheet1!$J$72,Sheet1!$J$83)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>289</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>429</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -708,13 +803,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="170567936"/>
-        <c:axId val="170573824"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="170567936"/>
+        <c:axId val="164423936"/>
+        <c:axId val="112381312"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="164423936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -748,15 +841,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170573824"/>
+        <c:crossAx val="112381312"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="170573824"/>
+        <c:axId val="112381312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -790,9 +880,9 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170567936"/>
+        <c:crossAx val="164423936"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -854,9 +944,6 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>10s</c:v>
-          </c:tx>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$E$12:$J$12</c:f>
@@ -886,20 +973,26 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$16:$H$16</c:f>
+              <c:f>Sheet1!$E$15:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>84</c:v>
+                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -910,9 +1003,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>20s</c:v>
-          </c:tx>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$E$42:$J$42</c:f>
@@ -942,27 +1032,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$46:$J$46</c:f>
+              <c:f>Sheet1!$E$45:$J$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>149</c:v>
+                  <c:v>394</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>89</c:v>
+                  <c:v>229</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -972,9 +1062,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:v>40s</c:v>
-          </c:tx>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$E$71:$J$71</c:f>
@@ -1004,27 +1091,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$75:$J$75</c:f>
+              <c:f>Sheet1!$E$74:$J$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>149</c:v>
+                  <c:v>404</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>149</c:v>
+                  <c:v>404</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>94</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1034,9 +1121,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="3"/>
-          <c:tx>
-            <c:v>60s</c:v>
-          </c:tx>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$E$82:$J$82</c:f>
@@ -1066,27 +1150,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$86:$J$86</c:f>
+              <c:f>Sheet1!$E$85:$J$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>149</c:v>
+                  <c:v>404</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>149</c:v>
+                  <c:v>404</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>114</c:v>
+                  <c:v>329</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>64</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1101,11 +1185,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="176974080"/>
-        <c:axId val="176972544"/>
+        <c:axId val="116222208"/>
+        <c:axId val="116224384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="176974080"/>
+        <c:axId val="116222208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1134,12 +1218,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="176972544"/>
+        <c:crossAx val="116224384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="176972544"/>
+        <c:axId val="116224384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1169,7 +1253,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="176974080"/>
+        <c:crossAx val="116222208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1311,7 +1395,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>149</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>84</c:v>
@@ -1361,7 +1445,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>149</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>119</c:v>
@@ -1411,10 +1495,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>149</c:v>
+                  <c:v>289</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>149</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>54</c:v>
@@ -1461,10 +1545,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>149</c:v>
+                  <c:v>429</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>149</c:v>
+                  <c:v>214</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>74</c:v>
@@ -1485,11 +1569,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="246013952"/>
-        <c:axId val="245999872"/>
+        <c:axId val="116269056"/>
+        <c:axId val="116270592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="246013952"/>
+        <c:axId val="116269056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1497,14 +1581,16 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="245999872"/>
+        <c:crossAx val="116270592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+        <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="245999872"/>
+        <c:axId val="116270592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1515,7 +1601,340 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="246013952"/>
+        <c:crossAx val="116269056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-BE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-BE"/>
+              <a:t>Possible stations in 16 TIM groups over various nr of slots</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$13:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$13:$S$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1520</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1440</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$43:$D$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$43:$S$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2640</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2720</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$61:$D$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$61:$S$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3840</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$72:$D$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$72:$S$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4640</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4960</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$83:$D$86</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$83:$S$86</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6880</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6880</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="105384960"/>
+        <c:axId val="157860608"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="105384960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="157860608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+        <c:minorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="157860608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="105384960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1597,15 +2016,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>571498</xdr:colOff>
-      <xdr:row>95</xdr:row>
-      <xdr:rowOff>68356</xdr:rowOff>
+      <xdr:colOff>179292</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>101973</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>593910</xdr:colOff>
-      <xdr:row>114</xdr:row>
-      <xdr:rowOff>145677</xdr:rowOff>
+      <xdr:colOff>201704</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1657,15 +2076,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>437030</xdr:colOff>
-      <xdr:row>113</xdr:row>
-      <xdr:rowOff>135591</xdr:rowOff>
+      <xdr:colOff>134471</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>169209</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>459441</xdr:colOff>
-      <xdr:row>139</xdr:row>
-      <xdr:rowOff>67235</xdr:rowOff>
+      <xdr:colOff>156882</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1679,6 +2098,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>134471</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>156882</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>10085</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1976,8 +2427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P105" sqref="P105"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77:S77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1986,27 +2437,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
       <c r="T1" s="24"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2171,17 +2622,17 @@
       <c r="D13" s="1">
         <v>1</v>
       </c>
-      <c r="E13">
-        <v>149</v>
-      </c>
-      <c r="F13">
-        <v>149</v>
+      <c r="E13" s="43">
+        <v>699</v>
+      </c>
+      <c r="F13" s="43">
+        <v>679</v>
       </c>
       <c r="G13">
-        <v>149</v>
+        <v>359</v>
       </c>
       <c r="H13">
-        <v>149</v>
+        <v>179</v>
       </c>
       <c r="I13">
         <v>124</v>
@@ -2193,27 +2644,27 @@
         <v>1</v>
       </c>
       <c r="N13">
-        <f>(E13+1)*$M13*N$12</f>
-        <v>150</v>
+        <f t="shared" ref="N13:S16" si="0">(E13+1)*$M13*N$12</f>
+        <v>700</v>
       </c>
       <c r="O13">
-        <f>(F13+1)*$M13*O$12</f>
-        <v>300</v>
+        <f t="shared" si="0"/>
+        <v>1360</v>
       </c>
       <c r="P13">
-        <f>(G13+1)*$M13*P$12</f>
-        <v>600</v>
+        <f t="shared" si="0"/>
+        <v>1440</v>
       </c>
       <c r="Q13">
-        <f>(H13+1)*$M13*Q$12</f>
-        <v>1200</v>
+        <f t="shared" si="0"/>
+        <v>1440</v>
       </c>
       <c r="R13">
-        <f>(I13+1)*$M13*R$12</f>
+        <f t="shared" si="0"/>
         <v>1500</v>
       </c>
       <c r="S13">
-        <f>(J13+1)*$M13*S$12</f>
+        <f t="shared" si="0"/>
         <v>1520</v>
       </c>
       <c r="V13" s="5" t="s">
@@ -2230,14 +2681,14 @@
       <c r="D14" s="1">
         <v>2</v>
       </c>
-      <c r="E14">
-        <v>149</v>
-      </c>
-      <c r="F14">
-        <v>149</v>
+      <c r="E14" s="43">
+        <v>584</v>
+      </c>
+      <c r="F14" s="43">
+        <v>349</v>
       </c>
       <c r="G14">
-        <v>149</v>
+        <v>184</v>
       </c>
       <c r="H14">
         <v>89</v>
@@ -2252,27 +2703,27 @@
         <v>2</v>
       </c>
       <c r="N14">
-        <f>(E14+1)*$M14*N$12</f>
-        <v>300</v>
+        <f t="shared" si="0"/>
+        <v>1170</v>
       </c>
       <c r="O14">
-        <f>(F14+1)*$M14*O$12</f>
-        <v>600</v>
+        <f t="shared" si="0"/>
+        <v>1400</v>
       </c>
       <c r="P14">
-        <f>(G14+1)*$M14*P$12</f>
-        <v>1200</v>
+        <f t="shared" si="0"/>
+        <v>1480</v>
       </c>
       <c r="Q14">
-        <f>(H14+1)*$M14*Q$12</f>
+        <f t="shared" si="0"/>
         <v>1440</v>
       </c>
       <c r="R14">
-        <f>(I14+1)*$M14*R$12</f>
+        <f t="shared" si="0"/>
         <v>1440</v>
       </c>
       <c r="S14">
-        <f>(J14+1)*$M14*S$12</f>
+        <f t="shared" si="0"/>
         <v>1440</v>
       </c>
       <c r="V14" s="5"/>
@@ -2285,8 +2736,8 @@
       <c r="D15" s="1">
         <v>5</v>
       </c>
-      <c r="E15">
-        <v>149</v>
+      <c r="E15" s="44">
+        <v>234</v>
       </c>
       <c r="F15">
         <v>119</v>
@@ -2307,27 +2758,27 @@
         <v>5</v>
       </c>
       <c r="N15">
-        <f>(E15+1)*$M15*N$12</f>
-        <v>750</v>
+        <f t="shared" si="0"/>
+        <v>1175</v>
       </c>
       <c r="O15">
-        <f>(F15+1)*$M15*O$12</f>
+        <f t="shared" si="0"/>
         <v>1200</v>
       </c>
       <c r="P15">
-        <f>(G15+1)*$M15*P$12</f>
+        <f t="shared" si="0"/>
         <v>1200</v>
       </c>
       <c r="Q15">
-        <f>(H15+1)*$M15*Q$12</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="R15">
-        <f>(I15+1)*$M15*R$12</f>
+        <f t="shared" si="0"/>
         <v>1200</v>
       </c>
       <c r="S15">
-        <f>(J15+1)*$M15*S$12</f>
+        <f t="shared" si="0"/>
         <v>800</v>
       </c>
       <c r="V15" s="8" t="s">
@@ -2347,7 +2798,7 @@
         <v>10</v>
       </c>
       <c r="E16">
-        <v>84</v>
+        <v>9</v>
       </c>
       <c r="F16">
         <v>39</v>
@@ -2359,36 +2810,36 @@
         <v>9</v>
       </c>
       <c r="I16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M16" s="1">
         <v>10</v>
       </c>
       <c r="N16">
-        <f>(E16+1)*$M16*N$12</f>
-        <v>850</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="O16">
-        <f>(F16+1)*$M16*O$12</f>
+        <f t="shared" si="0"/>
         <v>800</v>
       </c>
       <c r="P16">
-        <f>(G16+1)*$M16*P$12</f>
+        <f t="shared" si="0"/>
         <v>800</v>
       </c>
       <c r="Q16">
-        <f>(H16+1)*$M16*Q$12</f>
+        <f t="shared" si="0"/>
         <v>800</v>
       </c>
       <c r="R16" t="e">
-        <f>(I16+1)*$M16*R$12</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="S16" t="e">
-        <f>(J16+1)*$M16*S$12</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2418,15 +2869,15 @@
       <c r="D19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M19" s="26" t="s">
+      <c r="M19" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="N19" s="27"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="27"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="28"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="27"/>
       <c r="T19" s="6"/>
       <c r="V19" t="s">
         <v>23</v>
@@ -2450,20 +2901,20 @@
       </c>
     </row>
     <row r="20" spans="4:39" x14ac:dyDescent="0.25">
-      <c r="M20" s="29"/>
+      <c r="M20" s="28"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
-      <c r="S20" s="30"/>
+      <c r="S20" s="29"/>
       <c r="T20" s="6"/>
     </row>
     <row r="21" spans="4:39" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>0</v>
       </c>
-      <c r="M21" s="29"/>
+      <c r="M21" s="28"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6" t="s">
         <v>0</v>
@@ -2471,7 +2922,7 @@
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
-      <c r="S21" s="30"/>
+      <c r="S21" s="29"/>
       <c r="T21" s="6"/>
       <c r="V21" t="s">
         <v>25</v>
@@ -2516,7 +2967,7 @@
       <c r="J22" s="1">
         <v>16</v>
       </c>
-      <c r="M22" s="29" t="s">
+      <c r="M22" s="28" t="s">
         <v>1</v>
       </c>
       <c r="N22" s="16">
@@ -2534,7 +2985,7 @@
       <c r="R22" s="16">
         <v>12</v>
       </c>
-      <c r="S22" s="32">
+      <c r="S22" s="31">
         <v>16</v>
       </c>
       <c r="T22" s="6"/>
@@ -2561,7 +3012,7 @@
       <c r="J23">
         <v>1465</v>
       </c>
-      <c r="M23" s="31">
+      <c r="M23" s="30">
         <v>1</v>
       </c>
       <c r="N23" s="6">
@@ -2569,23 +3020,23 @@
         <v>4</v>
       </c>
       <c r="O23" s="6">
-        <f t="shared" ref="O23:S26" si="0">(3+1)*$M23*O$12</f>
+        <f t="shared" ref="O23:S26" si="1">(3+1)*$M23*O$12</f>
         <v>8</v>
       </c>
       <c r="P23" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="Q23" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="R23" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="S23" s="30">
-        <f t="shared" si="0"/>
+      <c r="S23" s="29">
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="T23" s="6"/>
@@ -2622,31 +3073,31 @@
       <c r="J24">
         <v>1483</v>
       </c>
-      <c r="M24" s="31">
+      <c r="M24" s="30">
         <v>2</v>
       </c>
       <c r="N24" s="6">
-        <f t="shared" ref="N24:N26" si="1">(3+1)*$M24*N$12</f>
+        <f t="shared" ref="N24:N26" si="2">(3+1)*$M24*N$12</f>
         <v>8</v>
       </c>
       <c r="O24" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="P24" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="Q24" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="R24" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="S24" s="30">
-        <f t="shared" si="0"/>
+      <c r="S24" s="29">
+        <f t="shared" si="1"/>
         <v>128</v>
       </c>
       <c r="T24" s="16"/>
@@ -2673,31 +3124,31 @@
       <c r="J25">
         <v>822</v>
       </c>
-      <c r="M25" s="31">
+      <c r="M25" s="30">
         <v>5</v>
       </c>
       <c r="N25" s="6">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O25" s="6">
         <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="O25" s="6">
-        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="P25" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="Q25" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>160</v>
       </c>
       <c r="R25" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
-      <c r="S25" s="30">
-        <f t="shared" si="0"/>
+      <c r="S25" s="29">
+        <f t="shared" si="1"/>
         <v>320</v>
       </c>
       <c r="T25" s="6"/>
@@ -2731,31 +3182,31 @@
       <c r="J26" t="s">
         <v>49</v>
       </c>
-      <c r="M26" s="33">
+      <c r="M26" s="32">
         <v>10</v>
       </c>
-      <c r="N26" s="34">
+      <c r="N26" s="33">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="O26" s="33">
         <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="O26" s="34">
-        <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="P26" s="34">
-        <f t="shared" si="0"/>
+      <c r="P26" s="33">
+        <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="Q26" s="34">
-        <f t="shared" si="0"/>
+      <c r="Q26" s="33">
+        <f t="shared" si="1"/>
         <v>320</v>
       </c>
-      <c r="R26" s="34">
-        <f t="shared" si="0"/>
+      <c r="R26" s="33">
+        <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="S26" s="35">
-        <f t="shared" si="0"/>
+      <c r="S26" s="34">
+        <f t="shared" si="1"/>
         <v>640</v>
       </c>
       <c r="T26" s="6"/>
@@ -2866,11 +3317,11 @@
         <v>1.3</v>
       </c>
       <c r="X31">
-        <f t="shared" ref="X31:X38" si="2">W31*1000/(1000*1000)*$Y$17</f>
+        <f t="shared" ref="X31:X38" si="3">W31*1000/(1000*1000)*$Y$17</f>
         <v>127.00999999999999</v>
       </c>
       <c r="Z31">
-        <f t="shared" ref="Z31:Z38" si="3">X31/($Y$5*$Y$15) * 1000*1000</f>
+        <f t="shared" ref="Z31:Z38" si="4">X31/($Y$5*$Y$15) * 1000*1000</f>
         <v>77.520751953125</v>
       </c>
       <c r="AC31" s="5" t="s">
@@ -2933,11 +3384,11 @@
         <v>1.95</v>
       </c>
       <c r="X32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>190.51499999999999</v>
       </c>
       <c r="Z32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>116.28112792968749</v>
       </c>
       <c r="AC32" s="18">
@@ -2948,15 +3399,15 @@
         <v>620.166015625</v>
       </c>
       <c r="AE32" s="20">
-        <f t="shared" ref="AE32:AG35" si="4">$Y$3*(500 + 162*5*120/$AC32)/($Y$15*AE$31)</f>
+        <f t="shared" ref="AE32:AG35" si="5">$Y$3*(500 + 162*5*120/$AC32)/($Y$15*AE$31)</f>
         <v>310.0830078125</v>
       </c>
       <c r="AF32" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>155.04150390625</v>
       </c>
       <c r="AG32" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>77.520751953125</v>
       </c>
       <c r="AI32" s="18">
@@ -2964,19 +3415,19 @@
       </c>
       <c r="AJ32" s="6">
         <f>(E13+1)*($Y$11*8/1024)/10</f>
-        <v>11.71875</v>
+        <v>54.6875</v>
       </c>
       <c r="AK32" s="6">
         <f>(F13+1)*($Y$11*8/1024)/10</f>
-        <v>11.71875</v>
+        <v>53.125</v>
       </c>
       <c r="AL32" s="6">
         <f>(G13+1)*($Y$11*8/1024)/10</f>
-        <v>11.71875</v>
+        <v>28.125</v>
       </c>
       <c r="AM32" s="7">
         <f>(H13+1)*($Y$11*8/1024)/10</f>
-        <v>11.71875</v>
+        <v>14.0625</v>
       </c>
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.25">
@@ -3008,49 +3459,49 @@
         <v>2.6</v>
       </c>
       <c r="X33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>254.01999999999998</v>
       </c>
       <c r="Z33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>155.04150390625</v>
       </c>
       <c r="AC33" s="18">
         <v>2</v>
       </c>
       <c r="AD33" s="20">
-        <f t="shared" ref="AD33:AD35" si="5">$Y$3*(500 + 162*5*120/$AC33)/($Y$15*AD$31)</f>
+        <f t="shared" ref="AD33:AD35" si="6">$Y$3*(500 + 162*5*120/$AC33)/($Y$15*AD$31)</f>
         <v>311.669921875</v>
       </c>
       <c r="AE33" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>155.8349609375</v>
       </c>
       <c r="AF33" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>77.91748046875</v>
       </c>
       <c r="AG33" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>38.958740234375</v>
       </c>
       <c r="AI33" s="18">
         <v>2</v>
       </c>
       <c r="AJ33" s="6">
-        <f t="shared" ref="AJ33:AJ35" si="6">(E14+1)*($Y$11*8/1024)/10</f>
-        <v>11.71875</v>
+        <f t="shared" ref="AJ33:AJ35" si="7">(E14+1)*($Y$11*8/1024)/10</f>
+        <v>45.703125</v>
       </c>
       <c r="AK33" s="6">
-        <f t="shared" ref="AK33:AK35" si="7">(F14+1)*($Y$11*8/1024)/10</f>
-        <v>11.71875</v>
+        <f t="shared" ref="AK33:AK35" si="8">(F14+1)*($Y$11*8/1024)/10</f>
+        <v>27.34375</v>
       </c>
       <c r="AL33" s="6">
-        <f t="shared" ref="AL33:AL35" si="8">(G14+1)*($Y$11*8/1024)/10</f>
-        <v>11.71875</v>
+        <f t="shared" ref="AL33:AL35" si="9">(G14+1)*($Y$11*8/1024)/10</f>
+        <v>14.453125</v>
       </c>
       <c r="AM33" s="7">
-        <f t="shared" ref="AM33:AM35" si="9">(H14+1)*($Y$11*8/1024)/10</f>
+        <f t="shared" ref="AM33:AM35" si="10">(H14+1)*($Y$11*8/1024)/10</f>
         <v>7.03125</v>
       </c>
     </row>
@@ -3083,49 +3534,49 @@
         <v>3.9</v>
       </c>
       <c r="X34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>381.03</v>
       </c>
       <c r="Z34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>232.56225585937497</v>
       </c>
       <c r="AC34" s="18">
         <v>5</v>
       </c>
       <c r="AD34" s="20">
+        <f t="shared" si="6"/>
+        <v>126.572265625</v>
+      </c>
+      <c r="AE34" s="20">
         <f t="shared" si="5"/>
-        <v>126.572265625</v>
-      </c>
-      <c r="AE34" s="20">
-        <f t="shared" si="4"/>
         <v>63.2861328125</v>
       </c>
       <c r="AF34" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>31.64306640625</v>
       </c>
       <c r="AG34" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>15.821533203125</v>
       </c>
       <c r="AI34" s="18">
         <v>5</v>
       </c>
       <c r="AJ34" s="6">
-        <f t="shared" si="6"/>
-        <v>11.71875</v>
+        <f t="shared" si="7"/>
+        <v>18.359375</v>
       </c>
       <c r="AK34" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9.375</v>
       </c>
       <c r="AL34" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.6875</v>
       </c>
       <c r="AM34" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.953125</v>
       </c>
     </row>
@@ -3137,49 +3588,49 @@
         <v>5.2</v>
       </c>
       <c r="X35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>508.03999999999996</v>
       </c>
       <c r="Z35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>310.0830078125</v>
       </c>
       <c r="AC35" s="19">
         <v>10</v>
       </c>
       <c r="AD35" s="22">
+        <f t="shared" si="6"/>
+        <v>64.873046875</v>
+      </c>
+      <c r="AE35" s="22">
         <f t="shared" si="5"/>
-        <v>64.873046875</v>
-      </c>
-      <c r="AE35" s="22">
-        <f t="shared" si="4"/>
         <v>32.4365234375</v>
       </c>
       <c r="AF35" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16.21826171875</v>
       </c>
       <c r="AG35" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.109130859375</v>
       </c>
       <c r="AI35" s="19">
         <v>10</v>
       </c>
       <c r="AJ35" s="9">
-        <f t="shared" si="6"/>
-        <v>6.640625</v>
+        <f t="shared" si="7"/>
+        <v>0.78125</v>
       </c>
       <c r="AK35" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.125</v>
       </c>
       <c r="AL35" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.5625</v>
       </c>
       <c r="AM35" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.78125</v>
       </c>
     </row>
@@ -3191,36 +3642,36 @@
         <v>5.8</v>
       </c>
       <c r="X36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>566.66</v>
       </c>
       <c r="Z36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>345.86181640624994</v>
       </c>
     </row>
     <row r="37" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="25"/>
-      <c r="O37" s="25"/>
-      <c r="P37" s="25"/>
-      <c r="Q37" s="25"/>
-      <c r="R37" s="25"/>
-      <c r="S37" s="25"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="42"/>
+      <c r="K37" s="42"/>
+      <c r="L37" s="42"/>
+      <c r="M37" s="42"/>
+      <c r="N37" s="42"/>
+      <c r="O37" s="42"/>
+      <c r="P37" s="42"/>
+      <c r="Q37" s="42"/>
+      <c r="R37" s="42"/>
+      <c r="S37" s="42"/>
       <c r="T37" s="24"/>
       <c r="V37">
         <v>7</v>
@@ -3229,11 +3680,11 @@
         <v>6.5</v>
       </c>
       <c r="X37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>635.04999999999995</v>
       </c>
       <c r="Z37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>387.60375976562494</v>
       </c>
     </row>
@@ -3245,11 +3696,11 @@
         <v>7.8</v>
       </c>
       <c r="X38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>762.06</v>
       </c>
       <c r="Z38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>465.12451171874994</v>
       </c>
     </row>
@@ -3402,50 +3853,50 @@
       <c r="D43" s="1">
         <v>1</v>
       </c>
-      <c r="E43">
-        <v>149</v>
-      </c>
-      <c r="F43">
-        <v>149</v>
-      </c>
-      <c r="G43">
-        <v>149</v>
+      <c r="E43" s="43">
+        <v>699</v>
+      </c>
+      <c r="F43" s="43">
+        <v>699</v>
+      </c>
+      <c r="G43" s="44">
+        <v>639</v>
       </c>
       <c r="H43">
-        <v>149</v>
+        <v>324</v>
       </c>
       <c r="I43">
-        <v>149</v>
+        <v>219</v>
       </c>
       <c r="J43">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="M43" s="1">
         <v>1</v>
       </c>
       <c r="N43">
-        <f>(E43+1)*$M43*N$12</f>
-        <v>150</v>
+        <f t="shared" ref="N43:S46" si="11">(E43+1)*$M43*N$12</f>
+        <v>700</v>
       </c>
       <c r="O43">
-        <f>(F43+1)*$M43*O$12</f>
-        <v>300</v>
+        <f t="shared" si="11"/>
+        <v>1400</v>
       </c>
       <c r="P43">
-        <f>(G43+1)*$M43*P$12</f>
-        <v>600</v>
+        <f t="shared" si="11"/>
+        <v>2560</v>
       </c>
       <c r="Q43">
-        <f>(H43+1)*$M43*Q$12</f>
-        <v>1200</v>
+        <f t="shared" si="11"/>
+        <v>2600</v>
       </c>
       <c r="R43">
-        <f>(I43+1)*$M43*R$12</f>
-        <v>1800</v>
+        <f t="shared" si="11"/>
+        <v>2640</v>
       </c>
       <c r="S43">
-        <f>(J43+1)*$M43*S$12</f>
-        <v>2400</v>
+        <f t="shared" si="11"/>
+        <v>2640</v>
       </c>
       <c r="W43" s="5" t="s">
         <v>32</v>
@@ -3480,36 +3931,36 @@
       </c>
       <c r="AJ43" s="6">
         <f>AJ32/AD32*100</f>
-        <v>1.8896149909455948</v>
+        <v>8.8182032910794419</v>
       </c>
       <c r="AK43" s="6">
-        <f t="shared" ref="AK43:AM43" si="10">AK32/AE32*100</f>
-        <v>3.7792299818911896</v>
+        <f t="shared" ref="AK43:AM43" si="12">AK32/AE32*100</f>
+        <v>17.132509251240062</v>
       </c>
       <c r="AL43" s="6">
-        <f t="shared" si="10"/>
-        <v>7.5584599637823793</v>
+        <f t="shared" si="12"/>
+        <v>18.140303913077709</v>
       </c>
       <c r="AM43" s="7">
-        <f t="shared" si="10"/>
-        <v>15.116919927564759</v>
+        <f t="shared" si="12"/>
+        <v>18.140303913077709</v>
       </c>
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.25">
       <c r="D44" s="1">
         <v>2</v>
       </c>
-      <c r="E44">
-        <v>149</v>
-      </c>
-      <c r="F44">
-        <v>149</v>
+      <c r="E44" s="43">
+        <v>694</v>
+      </c>
+      <c r="F44" s="43">
+        <v>659</v>
       </c>
       <c r="G44">
-        <v>149</v>
+        <v>329</v>
       </c>
       <c r="H44">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="I44">
         <v>119</v>
@@ -3521,27 +3972,27 @@
         <v>2</v>
       </c>
       <c r="N44">
-        <f>(E44+1)*$M44*N$12</f>
-        <v>300</v>
+        <f t="shared" si="11"/>
+        <v>1390</v>
       </c>
       <c r="O44">
-        <f>(F44+1)*$M44*O$12</f>
-        <v>600</v>
+        <f t="shared" si="11"/>
+        <v>2640</v>
       </c>
       <c r="P44">
-        <f>(G44+1)*$M44*P$12</f>
-        <v>1200</v>
+        <f t="shared" si="11"/>
+        <v>2640</v>
       </c>
       <c r="Q44">
-        <f>(H44+1)*$M44*Q$12</f>
-        <v>2400</v>
+        <f t="shared" si="11"/>
+        <v>2800</v>
       </c>
       <c r="R44">
-        <f>(I44+1)*$M44*R$12</f>
+        <f t="shared" si="11"/>
         <v>2880</v>
       </c>
       <c r="S44">
-        <f>(J44+1)*$M44*S$12</f>
+        <f t="shared" si="11"/>
         <v>2720</v>
       </c>
       <c r="W44" s="5" t="s">
@@ -3576,19 +4027,19 @@
         <v>2</v>
       </c>
       <c r="AJ44" s="6">
-        <f t="shared" ref="AJ44:AJ46" si="11">AJ33/AD33*100</f>
-        <v>3.7599874667084441</v>
+        <f t="shared" ref="AJ44:AJ46" si="13">AJ33/AD33*100</f>
+        <v>14.663951120162933</v>
       </c>
       <c r="AK44" s="6">
-        <f t="shared" ref="AK44:AK46" si="12">AK33/AE33*100</f>
-        <v>7.5199749334168882</v>
+        <f t="shared" ref="AK44:AK46" si="14">AK33/AE33*100</f>
+        <v>17.54660817797274</v>
       </c>
       <c r="AL44" s="6">
-        <f t="shared" ref="AL44:AL46" si="13">AL33/AF33*100</f>
-        <v>15.039949866833776</v>
+        <f t="shared" ref="AL44:AL46" si="15">AL33/AF33*100</f>
+        <v>18.549271502428326</v>
       </c>
       <c r="AM44" s="7">
-        <f t="shared" ref="AM44:AM46" si="14">AM33/AG33*100</f>
+        <f t="shared" ref="AM44:AM46" si="16">AM33/AG33*100</f>
         <v>18.047939840200534</v>
       </c>
     </row>
@@ -3597,10 +4048,10 @@
         <v>5</v>
       </c>
       <c r="E45">
-        <v>149</v>
+        <v>394</v>
       </c>
       <c r="F45">
-        <v>149</v>
+        <v>229</v>
       </c>
       <c r="G45">
         <v>119</v>
@@ -3618,27 +4069,27 @@
         <v>5</v>
       </c>
       <c r="N45">
-        <f>(E45+1)*$M45*N$12</f>
-        <v>750</v>
+        <f t="shared" si="11"/>
+        <v>1975</v>
       </c>
       <c r="O45">
-        <f>(F45+1)*$M45*O$12</f>
-        <v>1500</v>
+        <f t="shared" si="11"/>
+        <v>2300</v>
       </c>
       <c r="P45">
-        <f>(G45+1)*$M45*P$12</f>
+        <f t="shared" si="11"/>
         <v>2400</v>
       </c>
       <c r="Q45">
-        <f>(H45+1)*$M45*Q$12</f>
+        <f t="shared" si="11"/>
         <v>2400</v>
       </c>
       <c r="R45">
-        <f>(I45+1)*$M45*R$12</f>
+        <f t="shared" si="11"/>
         <v>2100</v>
       </c>
       <c r="S45">
-        <f>(J45+1)*$M45*S$12</f>
+        <f t="shared" si="11"/>
         <v>2000</v>
       </c>
       <c r="W45" s="5"/>
@@ -3655,19 +4106,19 @@
         <v>5</v>
       </c>
       <c r="AJ45" s="6">
-        <f t="shared" si="11"/>
-        <v>9.2585448653653266</v>
+        <f t="shared" si="13"/>
+        <v>14.505053622405677</v>
       </c>
       <c r="AK45" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>14.813671784584523</v>
       </c>
       <c r="AL45" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>14.813671784584523</v>
       </c>
       <c r="AM45" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>12.344726487153769</v>
       </c>
     </row>
@@ -3676,7 +4127,7 @@
         <v>10</v>
       </c>
       <c r="E46">
-        <v>149</v>
+        <v>9</v>
       </c>
       <c r="F46">
         <v>89</v>
@@ -3697,27 +4148,27 @@
         <v>10</v>
       </c>
       <c r="N46">
-        <f>(E46+1)*$M46*N$12</f>
-        <v>1500</v>
+        <f t="shared" si="11"/>
+        <v>100</v>
       </c>
       <c r="O46">
-        <f>(F46+1)*$M46*O$12</f>
+        <f t="shared" si="11"/>
         <v>1800</v>
       </c>
       <c r="P46">
-        <f>(G46+1)*$M46*P$12</f>
+        <f t="shared" si="11"/>
         <v>1600</v>
       </c>
       <c r="Q46">
-        <f>(H46+1)*$M46*Q$12</f>
+        <f t="shared" si="11"/>
         <v>1600</v>
       </c>
       <c r="R46">
-        <f>(I46+1)*$M46*R$12</f>
+        <f t="shared" si="11"/>
         <v>1800</v>
       </c>
       <c r="S46">
-        <f>(J46+1)*$M46*S$12</f>
+        <f t="shared" si="11"/>
         <v>1600</v>
       </c>
       <c r="W46" s="5"/>
@@ -3734,19 +4185,19 @@
         <v>10</v>
       </c>
       <c r="AJ46" s="9">
-        <f t="shared" si="11"/>
-        <v>10.236339003462291</v>
+        <f t="shared" si="13"/>
+        <v>1.2042751768779165</v>
       </c>
       <c r="AK46" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>9.6342014150233322</v>
       </c>
       <c r="AL46" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>9.6342014150233322</v>
       </c>
       <c r="AM46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>9.6342014150233322</v>
       </c>
     </row>
@@ -3900,11 +4351,11 @@
     </row>
     <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="D52" s="16"/>
-      <c r="E52" s="36"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="36"/>
-      <c r="I52" s="36"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="35"/>
       <c r="J52" s="6"/>
     </row>
     <row r="53" spans="1:33" x14ac:dyDescent="0.25">
@@ -3920,27 +4371,27 @@
       </c>
     </row>
     <row r="55" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A55" s="25" t="s">
+      <c r="A55" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
-      <c r="H55" s="25"/>
-      <c r="I55" s="25"/>
-      <c r="J55" s="25"/>
-      <c r="K55" s="25"/>
-      <c r="L55" s="25"/>
-      <c r="M55" s="25"/>
-      <c r="N55" s="25"/>
-      <c r="O55" s="25"/>
-      <c r="P55" s="25"/>
-      <c r="Q55" s="25"/>
-      <c r="R55" s="25"/>
-      <c r="S55" s="25"/>
+      <c r="B55" s="42"/>
+      <c r="C55" s="42"/>
+      <c r="D55" s="42"/>
+      <c r="E55" s="42"/>
+      <c r="F55" s="42"/>
+      <c r="G55" s="42"/>
+      <c r="H55" s="42"/>
+      <c r="I55" s="42"/>
+      <c r="J55" s="42"/>
+      <c r="K55" s="42"/>
+      <c r="L55" s="42"/>
+      <c r="M55" s="42"/>
+      <c r="N55" s="42"/>
+      <c r="O55" s="42"/>
+      <c r="P55" s="42"/>
+      <c r="Q55" s="42"/>
+      <c r="R55" s="42"/>
+      <c r="S55" s="42"/>
       <c r="T55" s="24"/>
     </row>
     <row r="57" spans="1:33" x14ac:dyDescent="0.25">
@@ -4005,70 +4456,70 @@
       <c r="D61" s="1">
         <v>1</v>
       </c>
-      <c r="E61">
-        <v>149</v>
-      </c>
-      <c r="F61">
-        <v>149</v>
-      </c>
-      <c r="G61">
-        <v>149</v>
+      <c r="E61" s="44">
+        <v>699</v>
+      </c>
+      <c r="F61" s="44">
+        <v>699</v>
+      </c>
+      <c r="G61" s="44">
+        <v>699</v>
       </c>
       <c r="H61">
-        <v>149</v>
+        <v>439</v>
       </c>
       <c r="I61">
-        <v>149</v>
+        <v>314</v>
       </c>
       <c r="J61">
-        <v>149</v>
+        <v>224</v>
       </c>
       <c r="M61" s="1">
         <v>1</v>
       </c>
       <c r="N61">
         <f>(E61+1)*$M61*Sheet1!N$12</f>
-        <v>150</v>
+        <v>700</v>
       </c>
       <c r="O61">
         <f>(F61+1)*$M61*Sheet1!O$12</f>
-        <v>300</v>
+        <v>1400</v>
       </c>
       <c r="P61">
         <f>(G61+1)*$M61*Sheet1!P$12</f>
-        <v>600</v>
+        <v>2800</v>
       </c>
       <c r="Q61">
         <f>(H61+1)*$M61*Sheet1!Q$12</f>
-        <v>1200</v>
+        <v>3520</v>
       </c>
       <c r="R61">
         <f>(I61+1)*$M61*Sheet1!R$12</f>
-        <v>1800</v>
+        <v>3780</v>
       </c>
       <c r="S61">
         <f>(J61+1)*$M61*Sheet1!S$12</f>
-        <v>2400</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="62" spans="1:33" x14ac:dyDescent="0.25">
       <c r="D62" s="1">
         <v>2</v>
       </c>
-      <c r="E62">
-        <v>149</v>
-      </c>
-      <c r="F62">
-        <v>149</v>
-      </c>
-      <c r="G62">
-        <v>149</v>
+      <c r="E62" s="44">
+        <v>699</v>
+      </c>
+      <c r="F62" s="44">
+        <v>699</v>
+      </c>
+      <c r="G62" s="44">
+        <v>474</v>
       </c>
       <c r="H62">
-        <v>149</v>
+        <v>234</v>
       </c>
       <c r="I62">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="J62">
         <v>119</v>
@@ -4078,23 +4529,23 @@
       </c>
       <c r="N62">
         <f>(E62+1)*$M62*Sheet1!N$12</f>
-        <v>300</v>
+        <v>1400</v>
       </c>
       <c r="O62">
         <f>(F62+1)*$M62*Sheet1!O$12</f>
-        <v>600</v>
+        <v>2800</v>
       </c>
       <c r="P62">
         <f>(G62+1)*$M62*Sheet1!P$12</f>
-        <v>1200</v>
+        <v>3800</v>
       </c>
       <c r="Q62">
         <f>(H62+1)*$M62*Sheet1!Q$12</f>
-        <v>2400</v>
+        <v>3760</v>
       </c>
       <c r="R62">
         <f>(I62+1)*$M62*Sheet1!R$12</f>
-        <v>3600</v>
+        <v>3720</v>
       </c>
       <c r="S62">
         <f>(J62+1)*$M62*Sheet1!S$12</f>
@@ -4106,13 +4557,13 @@
         <v>5</v>
       </c>
       <c r="E63">
-        <v>149</v>
+        <v>404</v>
       </c>
       <c r="F63">
-        <v>149</v>
+        <v>339</v>
       </c>
       <c r="G63">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="H63">
         <v>84</v>
@@ -4128,15 +4579,15 @@
       </c>
       <c r="N63">
         <f>(E63+1)*$M63*Sheet1!N$12</f>
-        <v>750</v>
+        <v>2025</v>
       </c>
       <c r="O63">
         <f>(F63+1)*$M63*Sheet1!O$12</f>
-        <v>1500</v>
+        <v>3400</v>
       </c>
       <c r="P63">
         <f>(G63+1)*$M63*Sheet1!P$12</f>
-        <v>3000</v>
+        <v>3400</v>
       </c>
       <c r="Q63">
         <f>(H63+1)*$M63*Sheet1!Q$12</f>
@@ -4156,13 +4607,13 @@
         <v>10</v>
       </c>
       <c r="E64">
-        <v>149</v>
+        <v>24</v>
       </c>
       <c r="F64">
         <v>129</v>
       </c>
       <c r="G64">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="H64">
         <v>34</v>
@@ -4178,7 +4629,7 @@
       </c>
       <c r="N64">
         <f>(E64+1)*$M64*Sheet1!N$12</f>
-        <v>1500</v>
+        <v>250</v>
       </c>
       <c r="O64">
         <f>(F64+1)*$M64*Sheet1!O$12</f>
@@ -4186,7 +4637,7 @@
       </c>
       <c r="P64">
         <f>(G64+1)*$M64*Sheet1!P$12</f>
-        <v>3400</v>
+        <v>2600</v>
       </c>
       <c r="Q64">
         <f>(H64+1)*$M64*Sheet1!Q$12</f>
@@ -4202,27 +4653,27 @@
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A66" s="25" t="s">
+      <c r="A66" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="25"/>
-      <c r="G66" s="25"/>
-      <c r="H66" s="25"/>
-      <c r="I66" s="25"/>
-      <c r="J66" s="25"/>
-      <c r="K66" s="25"/>
-      <c r="L66" s="25"/>
-      <c r="M66" s="25"/>
-      <c r="N66" s="25"/>
-      <c r="O66" s="25"/>
-      <c r="P66" s="25"/>
-      <c r="Q66" s="25"/>
-      <c r="R66" s="25"/>
-      <c r="S66" s="25"/>
+      <c r="B66" s="42"/>
+      <c r="C66" s="42"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="42"/>
+      <c r="I66" s="42"/>
+      <c r="J66" s="42"/>
+      <c r="K66" s="42"/>
+      <c r="L66" s="42"/>
+      <c r="M66" s="42"/>
+      <c r="N66" s="42"/>
+      <c r="O66" s="42"/>
+      <c r="P66" s="42"/>
+      <c r="Q66" s="42"/>
+      <c r="R66" s="42"/>
+      <c r="S66" s="42"/>
       <c r="T66" s="24"/>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
@@ -4287,100 +4738,100 @@
       <c r="D72" s="1">
         <v>1</v>
       </c>
-      <c r="E72">
-        <v>149</v>
-      </c>
-      <c r="F72">
-        <v>149</v>
-      </c>
-      <c r="G72">
-        <v>149</v>
-      </c>
-      <c r="H72">
-        <v>149</v>
+      <c r="E72" s="44">
+        <v>699</v>
+      </c>
+      <c r="F72" s="44">
+        <v>699</v>
+      </c>
+      <c r="G72" s="44">
+        <v>699</v>
+      </c>
+      <c r="H72" s="44">
+        <v>569</v>
       </c>
       <c r="I72">
-        <v>149</v>
+        <v>394</v>
       </c>
       <c r="J72">
-        <v>149</v>
+        <v>289</v>
       </c>
       <c r="M72" s="1">
         <v>1</v>
       </c>
       <c r="N72">
         <f>(E72+1)*$M72*Sheet1!N$12</f>
-        <v>150</v>
+        <v>700</v>
       </c>
       <c r="O72">
         <f>(F72+1)*$M72*Sheet1!O$12</f>
-        <v>300</v>
+        <v>1400</v>
       </c>
       <c r="P72">
         <f>(G72+1)*$M72*Sheet1!P$12</f>
-        <v>600</v>
+        <v>2800</v>
       </c>
       <c r="Q72">
         <f>(H72+1)*$M72*Sheet1!Q$12</f>
-        <v>1200</v>
+        <v>4560</v>
       </c>
       <c r="R72">
         <f>(I72+1)*$M72*Sheet1!R$12</f>
-        <v>1800</v>
+        <v>4740</v>
       </c>
       <c r="S72">
         <f>(J72+1)*$M72*Sheet1!S$12</f>
-        <v>2400</v>
+        <v>4640</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D73" s="1">
         <v>2</v>
       </c>
-      <c r="E73">
-        <v>149</v>
-      </c>
-      <c r="F73">
-        <v>149</v>
-      </c>
-      <c r="G73">
-        <v>149</v>
+      <c r="E73" s="44">
+        <v>699</v>
+      </c>
+      <c r="F73" s="44">
+        <v>699</v>
+      </c>
+      <c r="G73" s="44">
+        <v>629</v>
       </c>
       <c r="H73">
-        <v>149</v>
+        <v>309</v>
       </c>
       <c r="I73">
-        <v>149</v>
+        <v>204</v>
       </c>
       <c r="J73">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="M73" s="1">
         <v>2</v>
       </c>
       <c r="N73">
         <f>(E73+1)*$M73*Sheet1!N$12</f>
-        <v>300</v>
+        <v>1400</v>
       </c>
       <c r="O73">
         <f>(F73+1)*$M73*Sheet1!O$12</f>
-        <v>600</v>
+        <v>2800</v>
       </c>
       <c r="P73">
         <f>(G73+1)*$M73*Sheet1!P$12</f>
-        <v>1200</v>
+        <v>5040</v>
       </c>
       <c r="Q73">
         <f>(H73+1)*$M73*Sheet1!Q$12</f>
-        <v>2400</v>
+        <v>4960</v>
       </c>
       <c r="R73">
         <f>(I73+1)*$M73*Sheet1!R$12</f>
-        <v>3600</v>
+        <v>4920</v>
       </c>
       <c r="S73">
         <f>(J73+1)*$M73*Sheet1!S$12</f>
-        <v>4800</v>
+        <v>4960</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
@@ -4388,13 +4839,13 @@
         <v>5</v>
       </c>
       <c r="E74">
-        <v>149</v>
+        <v>404</v>
       </c>
       <c r="F74">
-        <v>149</v>
+        <v>404</v>
       </c>
       <c r="G74">
-        <v>149</v>
+        <v>224</v>
       </c>
       <c r="H74">
         <v>114</v>
@@ -4410,15 +4861,15 @@
       </c>
       <c r="N74">
         <f>(E74+1)*$M74*Sheet1!N$12</f>
-        <v>750</v>
+        <v>2025</v>
       </c>
       <c r="O74">
         <f>(F74+1)*$M74*Sheet1!O$12</f>
-        <v>1500</v>
+        <v>4050</v>
       </c>
       <c r="P74">
         <f>(G74+1)*$M74*Sheet1!P$12</f>
-        <v>3000</v>
+        <v>4500</v>
       </c>
       <c r="Q74">
         <f>(H74+1)*$M74*Sheet1!Q$12</f>
@@ -4438,9 +4889,9 @@
         <v>10</v>
       </c>
       <c r="E75">
-        <v>149</v>
-      </c>
-      <c r="F75">
+        <v>24</v>
+      </c>
+      <c r="F75" s="44">
         <v>149</v>
       </c>
       <c r="G75">
@@ -4460,7 +4911,7 @@
       </c>
       <c r="N75">
         <f>(E75+1)*$M75*Sheet1!N$12</f>
-        <v>1500</v>
+        <v>250</v>
       </c>
       <c r="O75">
         <f>(F75+1)*$M75*Sheet1!O$12</f>
@@ -4484,27 +4935,27 @@
       </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A77" s="25" t="s">
+      <c r="A77" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B77" s="25"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25"/>
-      <c r="E77" s="25"/>
-      <c r="F77" s="25"/>
-      <c r="G77" s="25"/>
-      <c r="H77" s="25"/>
-      <c r="I77" s="25"/>
-      <c r="J77" s="25"/>
-      <c r="K77" s="25"/>
-      <c r="L77" s="25"/>
-      <c r="M77" s="25"/>
-      <c r="N77" s="25"/>
-      <c r="O77" s="25"/>
-      <c r="P77" s="25"/>
-      <c r="Q77" s="25"/>
-      <c r="R77" s="25"/>
-      <c r="S77" s="25"/>
+      <c r="B77" s="42"/>
+      <c r="C77" s="42"/>
+      <c r="D77" s="42"/>
+      <c r="E77" s="42"/>
+      <c r="F77" s="42"/>
+      <c r="G77" s="42"/>
+      <c r="H77" s="42"/>
+      <c r="I77" s="42"/>
+      <c r="J77" s="42"/>
+      <c r="K77" s="42"/>
+      <c r="L77" s="42"/>
+      <c r="M77" s="42"/>
+      <c r="N77" s="42"/>
+      <c r="O77" s="42"/>
+      <c r="P77" s="42"/>
+      <c r="Q77" s="42"/>
+      <c r="R77" s="42"/>
+      <c r="S77" s="42"/>
       <c r="T77" s="24"/>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
@@ -4569,100 +5020,100 @@
       <c r="D83" s="1">
         <v>1</v>
       </c>
-      <c r="E83">
-        <v>149</v>
-      </c>
-      <c r="F83">
-        <v>149</v>
-      </c>
-      <c r="G83">
-        <v>149</v>
-      </c>
-      <c r="H83">
-        <v>149</v>
-      </c>
-      <c r="I83">
-        <v>149</v>
+      <c r="E83" s="44">
+        <v>699</v>
+      </c>
+      <c r="F83" s="44">
+        <v>699</v>
+      </c>
+      <c r="G83" s="44">
+        <v>699</v>
+      </c>
+      <c r="H83" s="43">
+        <v>694</v>
+      </c>
+      <c r="I83" s="44">
+        <v>454</v>
       </c>
       <c r="J83">
-        <v>149</v>
+        <v>429</v>
       </c>
       <c r="M83" s="1">
         <v>1</v>
       </c>
       <c r="N83">
         <f>(E83+1)*$M83*Sheet1!N$12</f>
-        <v>150</v>
+        <v>700</v>
       </c>
       <c r="O83">
         <f>(F83+1)*$M83*Sheet1!O$12</f>
-        <v>300</v>
+        <v>1400</v>
       </c>
       <c r="P83">
         <f>(G83+1)*$M83*Sheet1!P$12</f>
-        <v>600</v>
+        <v>2800</v>
       </c>
       <c r="Q83">
         <f>(H83+1)*$M83*Sheet1!Q$12</f>
-        <v>1200</v>
+        <v>5560</v>
       </c>
       <c r="R83">
         <f>(I83+1)*$M83*Sheet1!R$12</f>
-        <v>1800</v>
+        <v>5460</v>
       </c>
       <c r="S83">
         <f>(J83+1)*$M83*Sheet1!S$12</f>
-        <v>2400</v>
+        <v>6880</v>
       </c>
     </row>
     <row r="84" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D84" s="1">
         <v>2</v>
       </c>
-      <c r="E84">
-        <v>149</v>
-      </c>
-      <c r="F84">
-        <v>149</v>
-      </c>
-      <c r="G84">
-        <v>149</v>
+      <c r="E84" s="44">
+        <v>699</v>
+      </c>
+      <c r="F84" s="44">
+        <v>699</v>
+      </c>
+      <c r="G84" s="44">
+        <v>699</v>
       </c>
       <c r="H84">
-        <v>149</v>
+        <v>424</v>
       </c>
       <c r="I84">
-        <v>149</v>
+        <v>289</v>
       </c>
       <c r="J84">
-        <v>149</v>
+        <v>214</v>
       </c>
       <c r="M84" s="1">
         <v>2</v>
       </c>
       <c r="N84">
         <f>(E84+1)*$M84*Sheet1!N$12</f>
-        <v>300</v>
+        <v>1400</v>
       </c>
       <c r="O84">
         <f>(F84+1)*$M84*Sheet1!O$12</f>
-        <v>600</v>
+        <v>2800</v>
       </c>
       <c r="P84">
         <f>(G84+1)*$M84*Sheet1!P$12</f>
-        <v>1200</v>
+        <v>5600</v>
       </c>
       <c r="Q84">
         <f>(H84+1)*$M84*Sheet1!Q$12</f>
-        <v>2400</v>
+        <v>6800</v>
       </c>
       <c r="R84">
         <f>(I84+1)*$M84*Sheet1!R$12</f>
-        <v>3600</v>
+        <v>6960</v>
       </c>
       <c r="S84">
         <f>(J84+1)*$M84*Sheet1!S$12</f>
-        <v>4800</v>
+        <v>6880</v>
       </c>
     </row>
     <row r="85" spans="4:20" x14ac:dyDescent="0.25">
@@ -4670,16 +5121,16 @@
         <v>5</v>
       </c>
       <c r="E85">
-        <v>149</v>
+        <v>404</v>
       </c>
       <c r="F85">
-        <v>149</v>
+        <v>404</v>
       </c>
       <c r="G85">
-        <v>149</v>
+        <v>329</v>
       </c>
       <c r="H85">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="I85">
         <v>89</v>
@@ -4692,19 +5143,19 @@
       </c>
       <c r="N85">
         <f>(E85+1)*$M85*Sheet1!N$12</f>
-        <v>750</v>
+        <v>2025</v>
       </c>
       <c r="O85">
         <f>(F85+1)*$M85*Sheet1!O$12</f>
-        <v>1500</v>
+        <v>4050</v>
       </c>
       <c r="P85">
         <f>(G85+1)*$M85*Sheet1!P$12</f>
-        <v>3000</v>
+        <v>6600</v>
       </c>
       <c r="Q85">
         <f>(H85+1)*$M85*Sheet1!Q$12</f>
-        <v>6000</v>
+        <v>6600</v>
       </c>
       <c r="R85">
         <f>(I85+1)*$M85*Sheet1!R$12</f>
@@ -4720,13 +5171,13 @@
         <v>10</v>
       </c>
       <c r="E86">
-        <v>149</v>
+        <v>24</v>
       </c>
       <c r="F86">
         <v>149</v>
       </c>
       <c r="G86">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="H86">
         <v>64</v>
@@ -4742,7 +5193,7 @@
       </c>
       <c r="N86">
         <f>(E86+1)*$M86*Sheet1!N$12</f>
-        <v>1500</v>
+        <v>250</v>
       </c>
       <c r="O86">
         <f>(F86+1)*$M86*Sheet1!O$12</f>
@@ -4750,7 +5201,7 @@
       </c>
       <c r="P86">
         <f>(G86+1)*$M86*Sheet1!P$12</f>
-        <v>4600</v>
+        <v>5400</v>
       </c>
       <c r="Q86">
         <f>(H86+1)*$M86*Sheet1!Q$12</f>
@@ -4791,27 +5242,27 @@
       </c>
     </row>
     <row r="117" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B117" s="26" t="s">
+      <c r="B117" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C117" s="27"/>
-      <c r="D117" s="27"/>
-      <c r="E117" s="27"/>
-      <c r="F117" s="27"/>
-      <c r="G117" s="27"/>
-      <c r="H117" s="28"/>
+      <c r="C117" s="26"/>
+      <c r="D117" s="26"/>
+      <c r="E117" s="26"/>
+      <c r="F117" s="26"/>
+      <c r="G117" s="26"/>
+      <c r="H117" s="27"/>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B118" s="29"/>
+      <c r="B118" s="28"/>
       <c r="C118" s="6"/>
       <c r="D118" s="6"/>
       <c r="E118" s="6"/>
       <c r="F118" s="6"/>
       <c r="G118" s="6"/>
-      <c r="H118" s="30"/>
+      <c r="H118" s="29"/>
     </row>
     <row r="119" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B119" s="31" t="s">
+      <c r="B119" s="30" t="s">
         <v>2</v>
       </c>
       <c r="C119" s="6"/>
@@ -4819,19 +5270,19 @@
       <c r="E119" s="6"/>
       <c r="F119" s="6"/>
       <c r="G119" s="6"/>
-      <c r="H119" s="30"/>
+      <c r="H119" s="29"/>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B120" s="29"/>
+      <c r="B120" s="28"/>
       <c r="C120" s="6"/>
       <c r="D120" s="6"/>
       <c r="E120" s="6"/>
       <c r="F120" s="6"/>
       <c r="G120" s="6"/>
-      <c r="H120" s="30"/>
+      <c r="H120" s="29"/>
     </row>
     <row r="121" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B121" s="29"/>
+      <c r="B121" s="28"/>
       <c r="C121" s="6"/>
       <c r="D121" s="6" t="s">
         <v>0</v>
@@ -4839,10 +5290,10 @@
       <c r="E121" s="6"/>
       <c r="F121" s="6"/>
       <c r="G121" s="6"/>
-      <c r="H121" s="30"/>
+      <c r="H121" s="29"/>
     </row>
     <row r="122" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B122" s="29" t="s">
+      <c r="B122" s="28" t="s">
         <v>1</v>
       </c>
       <c r="C122" s="16">
@@ -4860,142 +5311,142 @@
       <c r="G122" s="16">
         <v>12</v>
       </c>
-      <c r="H122" s="32">
+      <c r="H122" s="31">
         <v>16</v>
       </c>
     </row>
     <row r="123" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B123" s="31">
+      <c r="B123" s="30">
         <v>1</v>
       </c>
       <c r="C123" s="6">
         <v>149</v>
       </c>
-      <c r="D123" s="36">
+      <c r="D123" s="35">
         <v>149</v>
       </c>
-      <c r="E123" s="36">
+      <c r="E123" s="35">
         <v>149</v>
       </c>
-      <c r="F123" s="36">
+      <c r="F123" s="35">
         <v>144</v>
       </c>
       <c r="G123" s="6">
         <v>94</v>
       </c>
-      <c r="H123" s="30">
+      <c r="H123" s="29">
         <v>74</v>
       </c>
     </row>
     <row r="124" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B124" s="31">
+      <c r="B124" s="30">
         <v>2</v>
       </c>
       <c r="C124" s="6">
         <v>149</v>
       </c>
-      <c r="D124" s="36">
+      <c r="D124" s="35">
         <v>149</v>
       </c>
-      <c r="E124" s="36">
+      <c r="E124" s="35">
         <v>134</v>
       </c>
-      <c r="F124" s="36">
+      <c r="F124" s="35">
         <v>64</v>
       </c>
       <c r="G124" s="6">
         <v>44</v>
       </c>
-      <c r="H124" s="30">
+      <c r="H124" s="29">
         <v>29</v>
       </c>
     </row>
     <row r="125" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B125" s="31">
+      <c r="B125" s="30">
         <v>5</v>
       </c>
-      <c r="C125" s="36">
+      <c r="C125" s="35">
         <v>149</v>
       </c>
-      <c r="D125" s="36">
+      <c r="D125" s="35">
         <v>84</v>
       </c>
-      <c r="E125" s="36">
+      <c r="E125" s="35">
         <v>39</v>
       </c>
-      <c r="F125" s="36">
+      <c r="F125" s="35">
         <v>19</v>
       </c>
-      <c r="G125" s="36">
+      <c r="G125" s="35">
         <v>14</v>
       </c>
-      <c r="H125" s="30">
+      <c r="H125" s="29">
         <v>9</v>
       </c>
     </row>
     <row r="126" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B126" s="33">
+      <c r="B126" s="32">
         <v>10</v>
       </c>
-      <c r="C126" s="34">
+      <c r="C126" s="33">
         <v>69</v>
       </c>
-      <c r="D126" s="34">
+      <c r="D126" s="33">
         <v>29</v>
       </c>
-      <c r="E126" s="34">
+      <c r="E126" s="33">
         <v>114</v>
       </c>
-      <c r="F126" s="34">
+      <c r="F126" s="33">
         <v>-1</v>
       </c>
-      <c r="G126" s="34">
+      <c r="G126" s="33">
         <v>-1</v>
       </c>
-      <c r="H126" s="35">
+      <c r="H126" s="34">
         <v>-1</v>
       </c>
     </row>
     <row r="129" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B129" s="26" t="s">
+      <c r="B129" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C129" s="27"/>
-      <c r="D129" s="27"/>
-      <c r="E129" s="27"/>
-      <c r="F129" s="27"/>
-      <c r="G129" s="27"/>
-      <c r="H129" s="28"/>
-      <c r="I129" s="27"/>
-      <c r="J129" s="26" t="s">
+      <c r="C129" s="26"/>
+      <c r="D129" s="26"/>
+      <c r="E129" s="26"/>
+      <c r="F129" s="26"/>
+      <c r="G129" s="26"/>
+      <c r="H129" s="27"/>
+      <c r="I129" s="26"/>
+      <c r="J129" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="K129" s="27"/>
-      <c r="L129" s="27"/>
-      <c r="M129" s="27"/>
-      <c r="N129" s="27"/>
-      <c r="O129" s="27"/>
-      <c r="P129" s="28"/>
+      <c r="K129" s="26"/>
+      <c r="L129" s="26"/>
+      <c r="M129" s="26"/>
+      <c r="N129" s="26"/>
+      <c r="O129" s="26"/>
+      <c r="P129" s="27"/>
     </row>
     <row r="130" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B130" s="29"/>
+      <c r="B130" s="28"/>
       <c r="C130" s="6"/>
       <c r="D130" s="6"/>
       <c r="E130" s="6"/>
       <c r="F130" s="6"/>
       <c r="G130" s="6"/>
-      <c r="H130" s="30"/>
+      <c r="H130" s="29"/>
       <c r="I130" s="6"/>
-      <c r="J130" s="29"/>
+      <c r="J130" s="28"/>
       <c r="K130" s="6"/>
       <c r="L130" s="6"/>
       <c r="M130" s="6"/>
       <c r="N130" s="6"/>
       <c r="O130" s="6"/>
-      <c r="P130" s="30"/>
+      <c r="P130" s="29"/>
     </row>
     <row r="131" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B131" s="31" t="s">
+      <c r="B131" s="30" t="s">
         <v>2</v>
       </c>
       <c r="C131" s="6"/>
@@ -5003,9 +5454,9 @@
       <c r="E131" s="6"/>
       <c r="F131" s="6"/>
       <c r="G131" s="6"/>
-      <c r="H131" s="30"/>
+      <c r="H131" s="29"/>
       <c r="I131" s="6"/>
-      <c r="J131" s="31" t="s">
+      <c r="J131" s="30" t="s">
         <v>2</v>
       </c>
       <c r="K131" s="6"/>
@@ -5013,27 +5464,27 @@
       <c r="M131" s="6"/>
       <c r="N131" s="6"/>
       <c r="O131" s="6"/>
-      <c r="P131" s="30"/>
+      <c r="P131" s="29"/>
     </row>
     <row r="132" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B132" s="29"/>
+      <c r="B132" s="28"/>
       <c r="C132" s="6"/>
       <c r="D132" s="6"/>
       <c r="E132" s="6"/>
       <c r="F132" s="6"/>
       <c r="G132" s="6"/>
-      <c r="H132" s="30"/>
+      <c r="H132" s="29"/>
       <c r="I132" s="6"/>
-      <c r="J132" s="29"/>
+      <c r="J132" s="28"/>
       <c r="K132" s="6"/>
       <c r="L132" s="6"/>
       <c r="M132" s="6"/>
       <c r="N132" s="6"/>
       <c r="O132" s="6"/>
-      <c r="P132" s="30"/>
+      <c r="P132" s="29"/>
     </row>
     <row r="133" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B133" s="29"/>
+      <c r="B133" s="28"/>
       <c r="C133" s="6"/>
       <c r="D133" s="6" t="s">
         <v>0</v>
@@ -5041,9 +5492,9 @@
       <c r="E133" s="6"/>
       <c r="F133" s="6"/>
       <c r="G133" s="6"/>
-      <c r="H133" s="30"/>
+      <c r="H133" s="29"/>
       <c r="I133" s="6"/>
-      <c r="J133" s="29"/>
+      <c r="J133" s="28"/>
       <c r="K133" s="6"/>
       <c r="L133" s="6" t="s">
         <v>0</v>
@@ -5051,10 +5502,10 @@
       <c r="M133" s="6"/>
       <c r="N133" s="6"/>
       <c r="O133" s="6"/>
-      <c r="P133" s="30"/>
+      <c r="P133" s="29"/>
     </row>
     <row r="134" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B134" s="29" t="s">
+      <c r="B134" s="28" t="s">
         <v>1</v>
       </c>
       <c r="C134" s="16">
@@ -5072,11 +5523,11 @@
       <c r="G134" s="16">
         <v>12</v>
       </c>
-      <c r="H134" s="32">
+      <c r="H134" s="31">
         <v>16</v>
       </c>
       <c r="I134" s="6"/>
-      <c r="J134" s="29" t="s">
+      <c r="J134" s="28" t="s">
         <v>1</v>
       </c>
       <c r="K134" s="16">
@@ -5094,34 +5545,34 @@
       <c r="O134" s="16">
         <v>12</v>
       </c>
-      <c r="P134" s="32">
+      <c r="P134" s="31">
         <v>16</v>
       </c>
     </row>
     <row r="135" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B135" s="31">
+      <c r="B135" s="30">
         <v>1</v>
       </c>
       <c r="C135" s="6">
         <v>149</v>
       </c>
-      <c r="D135" s="36">
+      <c r="D135" s="35">
         <v>149</v>
       </c>
-      <c r="E135" s="36">
+      <c r="E135" s="35">
         <v>149</v>
       </c>
-      <c r="F135" s="36">
+      <c r="F135" s="35">
         <v>149</v>
       </c>
       <c r="G135" s="6">
         <v>149</v>
       </c>
-      <c r="H135" s="30">
+      <c r="H135" s="29">
         <v>144</v>
       </c>
       <c r="I135" s="6"/>
-      <c r="J135" s="31">
+      <c r="J135" s="30">
         <v>1</v>
       </c>
       <c r="K135" s="6">
@@ -5139,34 +5590,34 @@
       <c r="O135" s="6">
         <v>124</v>
       </c>
-      <c r="P135" s="30">
+      <c r="P135" s="29">
         <v>94</v>
       </c>
     </row>
     <row r="136" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B136" s="31">
+      <c r="B136" s="30">
         <v>2</v>
       </c>
       <c r="C136" s="6">
         <v>149</v>
       </c>
-      <c r="D136" s="36">
+      <c r="D136" s="35">
         <v>149</v>
       </c>
-      <c r="E136" s="36">
+      <c r="E136" s="35">
         <v>149</v>
       </c>
-      <c r="F136" s="36">
+      <c r="F136" s="35">
         <v>134</v>
       </c>
       <c r="G136" s="6">
         <v>84</v>
       </c>
-      <c r="H136" s="30">
+      <c r="H136" s="29">
         <v>64</v>
       </c>
       <c r="I136" s="6"/>
-      <c r="J136" s="31">
+      <c r="J136" s="30">
         <v>2</v>
       </c>
       <c r="K136" s="6">
@@ -5184,34 +5635,34 @@
       <c r="O136" s="6">
         <v>59</v>
       </c>
-      <c r="P136" s="30">
+      <c r="P136" s="29">
         <v>44</v>
       </c>
     </row>
     <row r="137" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B137" s="31">
+      <c r="B137" s="30">
         <v>5</v>
       </c>
-      <c r="C137" s="36">
+      <c r="C137" s="35">
         <v>149</v>
       </c>
-      <c r="D137" s="36">
+      <c r="D137" s="35">
         <v>149</v>
       </c>
-      <c r="E137" s="36">
+      <c r="E137" s="35">
         <v>74</v>
       </c>
-      <c r="F137" s="36">
+      <c r="F137" s="35">
         <v>39</v>
       </c>
-      <c r="G137" s="36">
+      <c r="G137" s="35">
         <v>24</v>
       </c>
-      <c r="H137" s="30">
+      <c r="H137" s="29">
         <v>19</v>
       </c>
       <c r="I137" s="6"/>
-      <c r="J137" s="31">
+      <c r="J137" s="30">
         <v>5</v>
       </c>
       <c r="K137" s="6">
@@ -5229,77 +5680,77 @@
       <c r="O137" s="6">
         <v>19</v>
       </c>
-      <c r="P137" s="30">
+      <c r="P137" s="29">
         <v>9</v>
       </c>
     </row>
     <row r="138" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B138" s="33">
+      <c r="B138" s="32">
         <v>10</v>
       </c>
-      <c r="C138" s="34">
+      <c r="C138" s="33">
         <v>109</v>
       </c>
-      <c r="D138" s="34">
+      <c r="D138" s="33">
         <v>54</v>
       </c>
-      <c r="E138" s="34">
+      <c r="E138" s="33">
         <v>29</v>
       </c>
-      <c r="F138" s="34">
+      <c r="F138" s="33">
         <v>14</v>
       </c>
-      <c r="G138" s="34">
+      <c r="G138" s="33">
         <v>-1</v>
       </c>
-      <c r="H138" s="35">
+      <c r="H138" s="34">
         <v>-1</v>
       </c>
-      <c r="I138" s="34"/>
-      <c r="J138" s="33">
+      <c r="I138" s="33"/>
+      <c r="J138" s="32">
         <v>10</v>
       </c>
-      <c r="K138" s="34">
+      <c r="K138" s="33">
         <v>84</v>
       </c>
-      <c r="L138" s="34">
+      <c r="L138" s="33">
         <v>39</v>
       </c>
-      <c r="M138" s="34">
+      <c r="M138" s="33">
         <v>19</v>
       </c>
-      <c r="N138" s="34">
+      <c r="N138" s="33">
         <v>9</v>
       </c>
-      <c r="O138" s="34">
+      <c r="O138" s="33">
         <v>-1</v>
       </c>
-      <c r="P138" s="35">
+      <c r="P138" s="34">
         <v>-1</v>
       </c>
     </row>
     <row r="140" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F140" s="40" t="s">
+      <c r="F140" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="G140" s="41"/>
-      <c r="H140" s="41"/>
-      <c r="I140" s="41"/>
-      <c r="J140" s="41"/>
-      <c r="K140" s="41"/>
-      <c r="L140" s="42"/>
+      <c r="G140" s="40"/>
+      <c r="H140" s="40"/>
+      <c r="I140" s="40"/>
+      <c r="J140" s="40"/>
+      <c r="K140" s="40"/>
+      <c r="L140" s="41"/>
     </row>
     <row r="141" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F141" s="29"/>
+      <c r="F141" s="28"/>
       <c r="G141" s="6"/>
       <c r="H141" s="6"/>
       <c r="I141" s="6"/>
       <c r="J141" s="6"/>
       <c r="K141" s="6"/>
-      <c r="L141" s="30"/>
+      <c r="L141" s="29"/>
     </row>
     <row r="142" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F142" s="29"/>
+      <c r="F142" s="28"/>
       <c r="G142" s="6"/>
       <c r="H142" s="6" t="s">
         <v>0</v>
@@ -5307,10 +5758,10 @@
       <c r="I142" s="6"/>
       <c r="J142" s="6"/>
       <c r="K142" s="6"/>
-      <c r="L142" s="30"/>
+      <c r="L142" s="29"/>
     </row>
     <row r="143" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F143" s="29" t="s">
+      <c r="F143" s="28" t="s">
         <v>1</v>
       </c>
       <c r="G143" s="16">
@@ -5328,12 +5779,12 @@
       <c r="K143" s="16">
         <v>12</v>
       </c>
-      <c r="L143" s="32">
+      <c r="L143" s="31">
         <v>16</v>
       </c>
     </row>
     <row r="144" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F144" s="31">
+      <c r="F144" s="30">
         <v>1</v>
       </c>
       <c r="G144" s="20">
@@ -5341,106 +5792,106 @@
         <v>100</v>
       </c>
       <c r="H144" s="20">
-        <f t="shared" ref="H144:L144" si="15">D135/L135*100</f>
+        <f t="shared" ref="H144:L144" si="17">D135/L135*100</f>
         <v>100</v>
       </c>
       <c r="I144" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>100</v>
       </c>
       <c r="J144" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>100</v>
       </c>
       <c r="K144" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>120.16129032258065</v>
       </c>
-      <c r="L144" s="37">
-        <f t="shared" si="15"/>
+      <c r="L144" s="36">
+        <f t="shared" si="17"/>
         <v>153.19148936170214</v>
       </c>
     </row>
     <row r="145" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F145" s="31">
+      <c r="F145" s="30">
         <v>2</v>
       </c>
       <c r="G145" s="20">
-        <f t="shared" ref="G145:G147" si="16">C136/K136*100</f>
+        <f t="shared" ref="G145:G147" si="18">C136/K136*100</f>
         <v>100</v>
       </c>
       <c r="H145" s="20">
-        <f t="shared" ref="H145:H147" si="17">D136/L136*100</f>
+        <f t="shared" ref="H145:H147" si="19">D136/L136*100</f>
         <v>100</v>
       </c>
       <c r="I145" s="20">
-        <f t="shared" ref="I145:I147" si="18">E136/M136*100</f>
+        <f t="shared" ref="I145:I147" si="20">E136/M136*100</f>
         <v>100</v>
       </c>
       <c r="J145" s="20">
-        <f t="shared" ref="J145:J147" si="19">F136/N136*100</f>
+        <f t="shared" ref="J145:J147" si="21">F136/N136*100</f>
         <v>150.56179775280899</v>
       </c>
       <c r="K145" s="20">
-        <f t="shared" ref="K145:K146" si="20">G136/O136*100</f>
+        <f t="shared" ref="K145:K146" si="22">G136/O136*100</f>
         <v>142.37288135593221</v>
       </c>
-      <c r="L145" s="37">
-        <f t="shared" ref="L145:L146" si="21">H136/P136*100</f>
+      <c r="L145" s="36">
+        <f t="shared" ref="L145:L146" si="23">H136/P136*100</f>
         <v>145.45454545454547</v>
       </c>
     </row>
     <row r="146" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F146" s="31">
+      <c r="F146" s="30">
         <v>5</v>
       </c>
       <c r="G146" s="20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>100</v>
       </c>
       <c r="H146" s="20">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>125.21008403361344</v>
       </c>
       <c r="I146" s="20">
+        <f t="shared" si="20"/>
+        <v>125.42372881355932</v>
+      </c>
+      <c r="J146" s="20">
+        <f t="shared" si="21"/>
+        <v>162.5</v>
+      </c>
+      <c r="K146" s="20">
+        <f t="shared" si="22"/>
+        <v>126.31578947368421</v>
+      </c>
+      <c r="L146" s="36">
+        <f t="shared" si="23"/>
+        <v>211.11111111111111</v>
+      </c>
+    </row>
+    <row r="147" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F147" s="32">
+        <v>10</v>
+      </c>
+      <c r="G147" s="37">
         <f t="shared" si="18"/>
-        <v>125.42372881355932</v>
-      </c>
-      <c r="J146" s="20">
+        <v>129.76190476190476</v>
+      </c>
+      <c r="H147" s="37">
         <f t="shared" si="19"/>
-        <v>162.5</v>
-      </c>
-      <c r="K146" s="20">
+        <v>138.46153846153845</v>
+      </c>
+      <c r="I147" s="37">
         <f t="shared" si="20"/>
-        <v>126.31578947368421</v>
-      </c>
-      <c r="L146" s="37">
+        <v>152.63157894736844</v>
+      </c>
+      <c r="J147" s="37">
         <f t="shared" si="21"/>
-        <v>211.11111111111111</v>
-      </c>
-    </row>
-    <row r="147" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F147" s="33">
-        <v>10</v>
-      </c>
-      <c r="G147" s="38">
-        <f t="shared" si="16"/>
-        <v>129.76190476190476</v>
-      </c>
-      <c r="H147" s="38">
-        <f t="shared" si="17"/>
-        <v>138.46153846153845</v>
-      </c>
-      <c r="I147" s="38">
-        <f t="shared" si="18"/>
-        <v>152.63157894736844</v>
-      </c>
-      <c r="J147" s="38">
-        <f t="shared" si="19"/>
         <v>155.55555555555557</v>
       </c>
-      <c r="K147" s="38"/>
-      <c r="L147" s="39"/>
+      <c r="K147" s="37"/>
+      <c r="L147" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
updated docs & result files
</commit_message>
<xml_diff>
--- a/results/sensoranalysis.xlsx
+++ b/results/sensoranalysis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="58">
   <si>
     <t>Group</t>
   </si>
@@ -159,9 +159,6 @@
     <t>10 sec 100 bytes</t>
   </si>
   <si>
-    <t>Bigger payload difference % tov 10sec</t>
-  </si>
-  <si>
     <t>Max error</t>
   </si>
   <si>
@@ -178,6 +175,21 @@
   </si>
   <si>
     <t>30sec 300 bytes</t>
+  </si>
+  <si>
+    <t>40sec 400 bytes</t>
+  </si>
+  <si>
+    <t>16 TIM SLOT PAYLOAD INCREASE</t>
+  </si>
+  <si>
+    <t>200b  payload difference % tov 10sec</t>
+  </si>
+  <si>
+    <t>300b payload difference % tov 10sec</t>
+  </si>
+  <si>
+    <t>400b payload difference % tov 10sec</t>
   </si>
 </sst>
 </file>
@@ -479,7 +491,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -546,7 +558,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -600,7 +611,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -841,11 +851,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="143547776"/>
-        <c:axId val="143558144"/>
+        <c:axId val="145575296"/>
+        <c:axId val="145585664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="143547776"/>
+        <c:axId val="145575296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -872,19 +882,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143558144"/>
+        <c:crossAx val="145585664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="143558144"/>
+        <c:axId val="145585664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -911,21 +920,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143547776"/>
+        <c:crossAx val="145575296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -970,7 +977,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1223,11 +1229,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="146088320"/>
-        <c:axId val="146090240"/>
+        <c:axId val="148709760"/>
+        <c:axId val="148711680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="146088320"/>
+        <c:axId val="148709760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1249,19 +1255,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146090240"/>
+        <c:crossAx val="148711680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="146090240"/>
+        <c:axId val="148711680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1284,21 +1289,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146088320"/>
+        <c:crossAx val="148709760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1588,11 +1591,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="146143104"/>
-        <c:axId val="149819392"/>
+        <c:axId val="148764544"/>
+        <c:axId val="150474752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="146143104"/>
+        <c:axId val="148764544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1621,14 +1624,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149819392"/>
+        <c:crossAx val="150474752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149819392"/>
+        <c:axId val="150474752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1663,7 +1666,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146143104"/>
+        <c:crossAx val="148764544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1960,11 +1963,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="149861120"/>
-        <c:axId val="149863040"/>
+        <c:axId val="150506496"/>
+        <c:axId val="150520960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="149861120"/>
+        <c:axId val="150506496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1993,14 +1996,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149863040"/>
+        <c:crossAx val="150520960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149863040"/>
+        <c:axId val="150520960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2035,7 +2038,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149861120"/>
+        <c:crossAx val="150506496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2053,6 +2056,284 @@
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-BE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1 RAWslot</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$160:$B$163</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Sheet1!$H$135,Sheet1!$P$135,Sheet1!$X$135,Sheet1!$AF$135)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>194</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>2 RAWslots</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$160:$B$163</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Sheet1!$H$136,Sheet1!$P$136,Sheet1!$X$136,Sheet1!$AF$136)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>5 RAW slots</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$160:$B$163</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Sheet1!$H$137,Sheet1!$P$137,Sheet1!$X$137,Sheet1!$AF$137)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="151859584"/>
+        <c:axId val="151861504"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="151859584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Payload size and</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> traffic interval multiplier</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="151861504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="151861504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-BE" b="1"/>
+                  <a:t>Maximum attained contention</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="nl-BE" b="1" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="nl-BE" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="151859584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -2231,6 +2512,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>199060</xdr:colOff>
+      <xdr:row>193</xdr:row>
+      <xdr:rowOff>182250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2526,10 +2839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM162"/>
+  <dimension ref="A1:AM167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA130" sqref="AA130"/>
+    <sheetView tabSelected="1" topLeftCell="B122" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E154" sqref="E154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2911,10 +3224,10 @@
         <v>9</v>
       </c>
       <c r="I16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M16" s="1">
         <v>10</v>
@@ -2971,7 +3284,7 @@
         <v>4</v>
       </c>
       <c r="M19" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N19" s="26"/>
       <c r="O19" s="26"/>
@@ -3278,10 +3591,10 @@
         <v>597</v>
       </c>
       <c r="I26" s="42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J26" s="42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M26" s="32">
         <v>10</v>
@@ -3623,10 +3936,10 @@
         <v>96.08</v>
       </c>
       <c r="I34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V34">
         <v>4</v>
@@ -5508,9 +5821,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="129" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B129" s="25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C129" s="26"/>
       <c r="D129" s="26"/>
@@ -5520,7 +5833,7 @@
       <c r="H129" s="27"/>
       <c r="I129" s="26"/>
       <c r="J129" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K129" s="26"/>
       <c r="L129" s="26"/>
@@ -5529,7 +5842,7 @@
       <c r="O129" s="26"/>
       <c r="P129" s="27"/>
       <c r="R129" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S129" s="26"/>
       <c r="T129" s="26"/>
@@ -5537,8 +5850,17 @@
       <c r="V129" s="26"/>
       <c r="W129" s="26"/>
       <c r="X129" s="27"/>
-    </row>
-    <row r="130" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z129" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA129" s="26"/>
+      <c r="AB129" s="26"/>
+      <c r="AC129" s="26"/>
+      <c r="AD129" s="26"/>
+      <c r="AE129" s="26"/>
+      <c r="AF129" s="27"/>
+    </row>
+    <row r="130" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B130" s="28"/>
       <c r="C130" s="6"/>
       <c r="D130" s="6"/>
@@ -5561,8 +5883,15 @@
       <c r="V130" s="6"/>
       <c r="W130" s="6"/>
       <c r="X130" s="29"/>
-    </row>
-    <row r="131" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z130" s="28"/>
+      <c r="AA130" s="6"/>
+      <c r="AB130" s="6"/>
+      <c r="AC130" s="6"/>
+      <c r="AD130" s="6"/>
+      <c r="AE130" s="6"/>
+      <c r="AF130" s="29"/>
+    </row>
+    <row r="131" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B131" s="30" t="s">
         <v>2</v>
       </c>
@@ -5591,8 +5920,17 @@
       <c r="V131" s="6"/>
       <c r="W131" s="6"/>
       <c r="X131" s="29"/>
-    </row>
-    <row r="132" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z131" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA131" s="6"/>
+      <c r="AB131" s="6"/>
+      <c r="AC131" s="6"/>
+      <c r="AD131" s="6"/>
+      <c r="AE131" s="6"/>
+      <c r="AF131" s="29"/>
+    </row>
+    <row r="132" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B132" s="28"/>
       <c r="C132" s="6"/>
       <c r="D132" s="6"/>
@@ -5615,8 +5953,15 @@
       <c r="V132" s="6"/>
       <c r="W132" s="6"/>
       <c r="X132" s="29"/>
-    </row>
-    <row r="133" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z132" s="28"/>
+      <c r="AA132" s="6"/>
+      <c r="AB132" s="6"/>
+      <c r="AC132" s="6"/>
+      <c r="AD132" s="6"/>
+      <c r="AE132" s="6"/>
+      <c r="AF132" s="29"/>
+    </row>
+    <row r="133" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B133" s="28"/>
       <c r="C133" s="6"/>
       <c r="D133" s="6" t="s">
@@ -5645,8 +5990,17 @@
       <c r="V133" s="6"/>
       <c r="W133" s="6"/>
       <c r="X133" s="29"/>
-    </row>
-    <row r="134" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z133" s="28"/>
+      <c r="AA133" s="6"/>
+      <c r="AB133" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC133" s="6"/>
+      <c r="AD133" s="6"/>
+      <c r="AE133" s="6"/>
+      <c r="AF133" s="29"/>
+    </row>
+    <row r="134" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B134" s="28" t="s">
         <v>1</v>
       </c>
@@ -5711,45 +6065,66 @@
       <c r="X134" s="31">
         <v>16</v>
       </c>
-    </row>
-    <row r="135" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z134" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA134" s="16">
+        <v>1</v>
+      </c>
+      <c r="AB134" s="16">
+        <v>2</v>
+      </c>
+      <c r="AC134" s="16">
+        <v>4</v>
+      </c>
+      <c r="AD134" s="16">
+        <v>8</v>
+      </c>
+      <c r="AE134" s="16">
+        <v>12</v>
+      </c>
+      <c r="AF134" s="31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="135" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B135" s="30">
         <v>1</v>
       </c>
-      <c r="D135" s="44">
-        <v>634</v>
-      </c>
-      <c r="E135">
-        <v>544</v>
-      </c>
-      <c r="F135">
-        <v>264</v>
-      </c>
-      <c r="G135">
-        <v>184</v>
+      <c r="C135" s="48"/>
+      <c r="D135">
+        <v>679</v>
+      </c>
+      <c r="E135" s="6">
+        <v>359</v>
+      </c>
+      <c r="F135" s="6">
+        <v>179</v>
+      </c>
+      <c r="G135" s="6">
+        <v>124</v>
       </c>
       <c r="H135" s="29">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="I135" s="6"/>
       <c r="J135" s="30">
         <v>1</v>
       </c>
-      <c r="K135" s="48"/>
-      <c r="L135">
-        <v>679</v>
-      </c>
-      <c r="M135" s="6">
-        <v>359</v>
-      </c>
-      <c r="N135" s="6">
-        <v>179</v>
-      </c>
-      <c r="O135" s="6">
-        <v>124</v>
+      <c r="L135" s="44">
+        <v>634</v>
+      </c>
+      <c r="M135">
+        <v>544</v>
+      </c>
+      <c r="N135">
+        <v>264</v>
+      </c>
+      <c r="O135">
+        <v>184</v>
       </c>
       <c r="P135" s="29">
-        <v>94</v>
+        <v>144</v>
       </c>
       <c r="R135" s="30">
         <v>1</v>
@@ -5757,57 +6132,74 @@
       <c r="S135" s="48"/>
       <c r="T135" s="6"/>
       <c r="U135" s="6"/>
-      <c r="V135" s="6"/>
+      <c r="V135" s="6">
+        <v>319</v>
+      </c>
       <c r="W135" s="6">
         <v>229</v>
       </c>
       <c r="X135" s="29">
         <v>174</v>
       </c>
-    </row>
-    <row r="136" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z135" s="30">
+        <v>1</v>
+      </c>
+      <c r="AA135" s="48"/>
+      <c r="AB135" s="6"/>
+      <c r="AC135" s="6"/>
+      <c r="AD135" s="6">
+        <v>364</v>
+      </c>
+      <c r="AE135" s="6">
+        <v>254</v>
+      </c>
+      <c r="AF135" s="29">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="136" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B136" s="30">
         <v>2</v>
       </c>
-      <c r="C136" s="43">
-        <v>149</v>
-      </c>
-      <c r="D136">
-        <v>524</v>
-      </c>
-      <c r="E136">
-        <v>264</v>
-      </c>
-      <c r="F136" s="35">
-        <v>134</v>
+      <c r="C136">
+        <v>699</v>
+      </c>
+      <c r="D136" s="6">
+        <v>349</v>
+      </c>
+      <c r="E136" s="6">
+        <v>184</v>
+      </c>
+      <c r="F136" s="6">
+        <v>89</v>
       </c>
       <c r="G136" s="6">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="H136" s="29">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="I136" s="6"/>
       <c r="J136" s="30">
         <v>2</v>
       </c>
-      <c r="K136">
-        <v>699</v>
-      </c>
-      <c r="L136" s="6">
-        <v>349</v>
-      </c>
-      <c r="M136" s="6">
-        <v>184</v>
-      </c>
-      <c r="N136" s="6">
-        <v>89</v>
+      <c r="K136" s="43">
+        <v>149</v>
+      </c>
+      <c r="L136">
+        <v>524</v>
+      </c>
+      <c r="M136">
+        <v>264</v>
+      </c>
+      <c r="N136" s="35">
+        <v>134</v>
       </c>
       <c r="O136" s="6">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="P136" s="29">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="R136" s="30">
         <v>2</v>
@@ -5815,123 +6207,192 @@
       <c r="S136" s="6"/>
       <c r="T136" s="6"/>
       <c r="U136" s="6">
+        <v>309</v>
+      </c>
+      <c r="V136" s="6">
         <v>154</v>
       </c>
-      <c r="V136" s="6"/>
-      <c r="W136" s="6"/>
-      <c r="X136" s="29"/>
-    </row>
-    <row r="137" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="W136" s="6">
+        <v>99</v>
+      </c>
+      <c r="X136" s="29">
+        <v>79</v>
+      </c>
+      <c r="Z136" s="30">
+        <v>2</v>
+      </c>
+      <c r="AA136" s="6"/>
+      <c r="AB136" s="6"/>
+      <c r="AC136" s="6"/>
+      <c r="AD136" s="6">
+        <v>169</v>
+      </c>
+      <c r="AE136" s="6">
+        <v>109</v>
+      </c>
+      <c r="AF136" s="29">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="137" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B137" s="30">
         <v>5</v>
       </c>
-      <c r="C137">
-        <v>334</v>
-      </c>
-      <c r="D137">
-        <v>169</v>
-      </c>
-      <c r="E137" s="35">
-        <v>74</v>
-      </c>
-      <c r="F137" s="35">
-        <v>39</v>
-      </c>
-      <c r="G137" s="35">
+      <c r="C137" s="6">
+        <v>234</v>
+      </c>
+      <c r="D137" s="6">
+        <v>119</v>
+      </c>
+      <c r="E137" s="6">
+        <v>59</v>
+      </c>
+      <c r="F137" s="6">
         <v>24</v>
       </c>
+      <c r="G137" s="6">
+        <v>19</v>
+      </c>
       <c r="H137" s="29">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="I137" s="6"/>
       <c r="J137" s="30">
         <v>5</v>
       </c>
-      <c r="K137" s="6">
-        <v>234</v>
-      </c>
-      <c r="L137" s="6">
-        <v>119</v>
-      </c>
-      <c r="M137" s="6">
-        <v>59</v>
-      </c>
-      <c r="N137" s="6">
+      <c r="K137">
+        <v>334</v>
+      </c>
+      <c r="L137">
+        <v>169</v>
+      </c>
+      <c r="M137" s="35">
+        <v>74</v>
+      </c>
+      <c r="N137" s="35">
+        <v>39</v>
+      </c>
+      <c r="O137" s="35">
         <v>24</v>
       </c>
-      <c r="O137" s="6">
+      <c r="P137" s="29">
         <v>19</v>
-      </c>
-      <c r="P137" s="29">
-        <v>9</v>
       </c>
       <c r="R137" s="30">
         <v>5</v>
       </c>
       <c r="S137" s="6"/>
       <c r="T137" s="6"/>
-      <c r="U137" s="6"/>
-      <c r="V137" s="6"/>
-      <c r="W137" s="6"/>
-      <c r="X137" s="29"/>
-    </row>
-    <row r="138" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="U137" s="6">
+        <v>84</v>
+      </c>
+      <c r="V137" s="6">
+        <v>39</v>
+      </c>
+      <c r="W137" s="6">
+        <v>24</v>
+      </c>
+      <c r="X137" s="29">
+        <v>19</v>
+      </c>
+      <c r="Z137" s="30">
+        <v>5</v>
+      </c>
+      <c r="AA137" s="6"/>
+      <c r="AB137" s="6"/>
+      <c r="AC137" s="6"/>
+      <c r="AD137" s="35">
+        <v>44</v>
+      </c>
+      <c r="AE137" s="35">
+        <v>29</v>
+      </c>
+      <c r="AF137" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="138" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B138" s="32">
         <v>10</v>
       </c>
       <c r="C138" s="33">
-        <v>109</v>
+        <v>9</v>
       </c>
       <c r="D138" s="33">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="E138" s="33">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F138" s="33">
-        <v>14</v>
-      </c>
-      <c r="G138" s="33">
-        <v>-1</v>
-      </c>
-      <c r="H138" s="34">
-        <v>-1</v>
+        <v>9</v>
+      </c>
+      <c r="G138" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="H138" s="34" t="s">
+        <v>51</v>
       </c>
       <c r="I138" s="33"/>
       <c r="J138" s="32">
         <v>10</v>
       </c>
       <c r="K138" s="33">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="L138" s="33">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="M138" s="33">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="N138" s="33">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="O138" s="33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="P138" s="34" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R138" s="32">
         <v>10</v>
       </c>
       <c r="S138" s="33"/>
       <c r="T138" s="33"/>
-      <c r="U138" s="33"/>
-      <c r="V138" s="33"/>
-      <c r="W138" s="33"/>
-      <c r="X138" s="34"/>
-    </row>
-    <row r="140" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="U138" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="V138" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="W138" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="X138" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z138" s="32">
+        <v>10</v>
+      </c>
+      <c r="AA138" s="33"/>
+      <c r="AB138" s="33"/>
+      <c r="AC138" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD138" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE138" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF138" s="34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="140" spans="2:32" x14ac:dyDescent="0.25">
       <c r="F140" s="39" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="G140" s="40"/>
       <c r="H140" s="40"/>
@@ -5940,7 +6401,7 @@
       <c r="K140" s="40"/>
       <c r="L140" s="41"/>
     </row>
-    <row r="141" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:32" x14ac:dyDescent="0.25">
       <c r="F141" s="28"/>
       <c r="G141" s="6"/>
       <c r="H141" s="6"/>
@@ -5949,7 +6410,7 @@
       <c r="K141" s="6"/>
       <c r="L141" s="29"/>
     </row>
-    <row r="142" spans="2:24" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:32" ht="23.25" x14ac:dyDescent="0.25">
       <c r="F142" s="28"/>
       <c r="G142" s="6"/>
       <c r="H142" s="6" t="s">
@@ -5960,10 +6421,10 @@
       <c r="K142" s="6"/>
       <c r="L142" s="29"/>
       <c r="X142" s="45" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="143" spans="2:24" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="143" spans="2:32" x14ac:dyDescent="0.25">
       <c r="F143" s="28" t="s">
         <v>1</v>
       </c>
@@ -5986,18 +6447,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="144" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:32" x14ac:dyDescent="0.25">
       <c r="F144" s="30">
         <v>1</v>
       </c>
       <c r="G144" s="49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H144" s="49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I144" s="20">
-        <f t="shared" ref="I144:L144" si="17">E135/M135*100</f>
+        <f t="shared" ref="I144:L146" si="17">M135/E135*100</f>
         <v>151.53203342618383</v>
       </c>
       <c r="J144" s="20">
@@ -6013,192 +6474,442 @@
         <v>153.19148936170214</v>
       </c>
     </row>
-    <row r="145" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F145" s="30">
         <v>2</v>
       </c>
       <c r="G145" s="49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H145" s="20">
-        <f t="shared" ref="H145:H147" si="18">D136/L136*100</f>
+        <f>L136/D136*100</f>
         <v>150.14326647564471</v>
       </c>
       <c r="I145" s="20">
-        <f t="shared" ref="I145:I147" si="19">E136/M136*100</f>
+        <f t="shared" si="17"/>
         <v>143.47826086956522</v>
       </c>
       <c r="J145" s="20">
-        <f t="shared" ref="J145:J147" si="20">F136/N136*100</f>
+        <f t="shared" si="17"/>
         <v>150.56179775280899</v>
       </c>
       <c r="K145" s="20">
-        <f t="shared" ref="K145:K146" si="21">G136/O136*100</f>
+        <f t="shared" si="17"/>
         <v>142.37288135593221</v>
       </c>
       <c r="L145" s="36">
-        <f t="shared" ref="L145:L146" si="22">H136/P136*100</f>
+        <f t="shared" si="17"/>
         <v>145.45454545454547</v>
       </c>
     </row>
-    <row r="146" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F146" s="30">
         <v>5</v>
       </c>
       <c r="G146" s="20">
-        <f t="shared" ref="G146:G147" si="23">C137/K137*100</f>
+        <f>K137/C137*100</f>
         <v>142.73504273504273</v>
       </c>
       <c r="H146" s="20">
-        <f t="shared" si="18"/>
+        <f>L137/D137*100</f>
         <v>142.01680672268907</v>
       </c>
       <c r="I146" s="20">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>125.42372881355932</v>
       </c>
       <c r="J146" s="20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>162.5</v>
       </c>
       <c r="K146" s="20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>126.31578947368421</v>
       </c>
       <c r="L146" s="36">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>211.11111111111111</v>
       </c>
     </row>
-    <row r="147" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F147" s="32">
         <v>10</v>
       </c>
       <c r="G147" s="37">
-        <f t="shared" si="23"/>
+        <f>K138/C138*100</f>
         <v>1211.1111111111111</v>
       </c>
       <c r="H147" s="37">
-        <f t="shared" si="18"/>
+        <f>L138/D138*100</f>
         <v>138.46153846153845</v>
       </c>
       <c r="I147" s="37">
-        <f t="shared" si="19"/>
+        <f>M138/E138*100</f>
         <v>152.63157894736844</v>
       </c>
       <c r="J147" s="37">
-        <f t="shared" si="20"/>
+        <f>N138/F138*100</f>
         <v>155.55555555555557</v>
       </c>
       <c r="K147" s="37"/>
       <c r="L147" s="38"/>
     </row>
-    <row r="152" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C152">
-        <f>K135*1.7</f>
+    <row r="150" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F150" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="G150" s="40"/>
+      <c r="H150" s="40"/>
+      <c r="I150" s="40"/>
+      <c r="J150" s="40"/>
+      <c r="K150" s="40"/>
+      <c r="L150" s="41"/>
+    </row>
+    <row r="151" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F151" s="28"/>
+      <c r="G151" s="6"/>
+      <c r="H151" s="6"/>
+      <c r="I151" s="6"/>
+      <c r="J151" s="6"/>
+      <c r="K151" s="6"/>
+      <c r="L151" s="29"/>
+    </row>
+    <row r="152" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F152" s="28"/>
+      <c r="G152" s="6"/>
+      <c r="H152" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D152">
-        <f t="shared" ref="D152:H152" si="24">L135*1.7</f>
-        <v>1154.3</v>
-      </c>
-      <c r="E152">
+      <c r="I152" s="6"/>
+      <c r="J152" s="6"/>
+      <c r="K152" s="6"/>
+      <c r="L152" s="29"/>
+    </row>
+    <row r="153" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F153" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G153" s="16">
+        <v>1</v>
+      </c>
+      <c r="H153" s="16">
+        <v>2</v>
+      </c>
+      <c r="I153" s="16">
+        <v>4</v>
+      </c>
+      <c r="J153" s="16">
+        <v>8</v>
+      </c>
+      <c r="K153" s="16">
+        <v>12</v>
+      </c>
+      <c r="L153" s="31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="154" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F154" s="30">
+        <v>1</v>
+      </c>
+      <c r="G154" s="20" t="e">
+        <f t="shared" ref="G154:L157" si="18">S135/C135*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H154" s="20">
+        <f>T135/D135*100</f>
+        <v>0</v>
+      </c>
+      <c r="I154" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="J154" s="20">
+        <f t="shared" si="18"/>
+        <v>178.21229050279331</v>
+      </c>
+      <c r="K154" s="20">
+        <f t="shared" si="18"/>
+        <v>184.67741935483869</v>
+      </c>
+      <c r="L154" s="20">
+        <f t="shared" si="18"/>
+        <v>185.10638297872339</v>
+      </c>
+    </row>
+    <row r="155" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F155" s="30">
+        <v>2</v>
+      </c>
+      <c r="G155" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="H155" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="I155" s="20">
+        <f t="shared" si="18"/>
+        <v>167.93478260869566</v>
+      </c>
+      <c r="J155" s="20">
+        <f t="shared" si="18"/>
+        <v>173.03370786516854</v>
+      </c>
+      <c r="K155" s="20">
+        <f t="shared" si="18"/>
+        <v>167.79661016949152</v>
+      </c>
+      <c r="L155" s="20">
+        <f t="shared" si="18"/>
+        <v>179.54545454545453</v>
+      </c>
+    </row>
+    <row r="156" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F156" s="30">
+        <v>5</v>
+      </c>
+      <c r="G156" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="H156" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="I156" s="20">
+        <f t="shared" si="18"/>
+        <v>142.37288135593221</v>
+      </c>
+      <c r="J156" s="20">
+        <f t="shared" si="18"/>
+        <v>162.5</v>
+      </c>
+      <c r="K156" s="20">
+        <f t="shared" si="18"/>
+        <v>126.31578947368421</v>
+      </c>
+      <c r="L156" s="20">
+        <f t="shared" si="18"/>
+        <v>211.11111111111111</v>
+      </c>
+    </row>
+    <row r="157" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F157" s="32">
+        <v>10</v>
+      </c>
+      <c r="G157" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="H157" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="I157" s="20" t="e">
+        <f t="shared" si="18"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J157" s="20" t="e">
+        <f t="shared" si="18"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K157" s="20" t="e">
+        <f t="shared" si="18"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L157" s="20" t="e">
+        <f t="shared" si="18"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="159" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F159" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="G159" s="40"/>
+      <c r="H159" s="40"/>
+      <c r="I159" s="40"/>
+      <c r="J159" s="40"/>
+      <c r="K159" s="40"/>
+      <c r="L159" s="41"/>
+    </row>
+    <row r="160" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B160">
+        <v>1</v>
+      </c>
+      <c r="F160" s="28"/>
+      <c r="G160" s="6"/>
+      <c r="H160" s="6"/>
+      <c r="I160" s="6"/>
+      <c r="J160" s="6"/>
+      <c r="K160" s="6"/>
+      <c r="L160" s="29"/>
+    </row>
+    <row r="161" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B161">
+        <v>2</v>
+      </c>
+      <c r="F161" s="28"/>
+      <c r="G161" s="6"/>
+      <c r="H161" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I161" s="6"/>
+      <c r="J161" s="6"/>
+      <c r="K161" s="6"/>
+      <c r="L161" s="29"/>
+    </row>
+    <row r="162" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B162">
+        <v>3</v>
+      </c>
+      <c r="F162" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G162" s="16">
+        <v>1</v>
+      </c>
+      <c r="H162" s="16">
+        <v>2</v>
+      </c>
+      <c r="I162" s="16">
+        <v>4</v>
+      </c>
+      <c r="J162" s="16">
+        <v>8</v>
+      </c>
+      <c r="K162" s="16">
+        <v>12</v>
+      </c>
+      <c r="L162" s="31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="163" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B163">
+        <v>4</v>
+      </c>
+      <c r="F163" s="30">
+        <v>1</v>
+      </c>
+      <c r="G163" s="20" t="e">
+        <f>AA135/C135*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H163" s="20">
+        <f t="shared" ref="H163:L163" si="19">AB135/D135*100</f>
+        <v>0</v>
+      </c>
+      <c r="I163" s="20">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J163" s="20">
+        <f t="shared" si="19"/>
+        <v>203.35195530726256</v>
+      </c>
+      <c r="K163" s="20">
+        <f t="shared" si="19"/>
+        <v>204.83870967741936</v>
+      </c>
+      <c r="L163" s="20">
+        <f t="shared" si="19"/>
+        <v>206.38297872340425</v>
+      </c>
+    </row>
+    <row r="164" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F164" s="30">
+        <v>2</v>
+      </c>
+      <c r="G164" s="20">
+        <f t="shared" ref="G164:G166" si="20">AA136/C136*100</f>
+        <v>0</v>
+      </c>
+      <c r="H164" s="20">
+        <f t="shared" ref="H164:H166" si="21">AB136/D136*100</f>
+        <v>0</v>
+      </c>
+      <c r="I164" s="20">
+        <f t="shared" ref="I164:I166" si="22">AC136/E136*100</f>
+        <v>0</v>
+      </c>
+      <c r="J164" s="20">
+        <f t="shared" ref="J164:J166" si="23">AD136/F136*100</f>
+        <v>189.88764044943821</v>
+      </c>
+      <c r="K164" s="20">
+        <f t="shared" ref="K164:K166" si="24">AE136/G136*100</f>
+        <v>184.74576271186442</v>
+      </c>
+      <c r="L164" s="20">
+        <f t="shared" ref="L164:L166" si="25">AF136/H136*100</f>
+        <v>179.54545454545453</v>
+      </c>
+    </row>
+    <row r="165" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F165" s="30">
+        <v>5</v>
+      </c>
+      <c r="G165" s="20">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="H165" s="20">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="I165" s="20">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="J165" s="20">
+        <f t="shared" si="23"/>
+        <v>183.33333333333331</v>
+      </c>
+      <c r="K165" s="20">
         <f t="shared" si="24"/>
-        <v>610.29999999999995</v>
-      </c>
-      <c r="F152">
+        <v>152.63157894736844</v>
+      </c>
+      <c r="L165" s="20">
+        <f t="shared" si="25"/>
+        <v>211.11111111111111</v>
+      </c>
+    </row>
+    <row r="166" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F166" s="32">
+        <v>10</v>
+      </c>
+      <c r="G166" s="20">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="H166" s="20">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="I166" s="20" t="e">
+        <f t="shared" si="22"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J166" s="20" t="e">
+        <f t="shared" si="23"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K166" s="20" t="e">
         <f t="shared" si="24"/>
-        <v>304.3</v>
-      </c>
-      <c r="G152">
-        <f t="shared" si="24"/>
-        <v>210.79999999999998</v>
-      </c>
-      <c r="H152">
-        <f t="shared" si="24"/>
-        <v>159.79999999999998</v>
-      </c>
-    </row>
-    <row r="153" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C153">
-        <f t="shared" ref="C153:C155" si="25">K136*1.7</f>
-        <v>1188.3</v>
-      </c>
-      <c r="D153">
-        <f t="shared" ref="D153:D155" si="26">L136*1.7</f>
-        <v>593.29999999999995</v>
-      </c>
-      <c r="E153">
-        <f t="shared" ref="E153:E155" si="27">M136*1.7</f>
-        <v>312.8</v>
-      </c>
-      <c r="F153">
-        <f t="shared" ref="F153:F155" si="28">N136*1.7</f>
-        <v>151.29999999999998</v>
-      </c>
-      <c r="G153">
-        <f t="shared" ref="G153:G155" si="29">O136*1.7</f>
-        <v>100.3</v>
-      </c>
-      <c r="H153">
-        <f t="shared" ref="H153:H155" si="30">P136*1.7</f>
-        <v>74.8</v>
-      </c>
-    </row>
-    <row r="154" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C154">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L166" s="20" t="e">
         <f t="shared" si="25"/>
-        <v>397.8</v>
-      </c>
-      <c r="D154">
-        <f t="shared" si="26"/>
-        <v>202.29999999999998</v>
-      </c>
-      <c r="E154">
-        <f t="shared" si="27"/>
-        <v>100.3</v>
-      </c>
-      <c r="F154">
-        <f t="shared" si="28"/>
-        <v>40.799999999999997</v>
-      </c>
-      <c r="G154">
-        <f t="shared" si="29"/>
-        <v>32.299999999999997</v>
-      </c>
-      <c r="H154">
-        <f t="shared" si="30"/>
-        <v>15.299999999999999</v>
-      </c>
-    </row>
-    <row r="155" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C155">
-        <f t="shared" si="25"/>
-        <v>15.299999999999999</v>
-      </c>
-      <c r="D155">
-        <f t="shared" si="26"/>
-        <v>66.3</v>
-      </c>
-      <c r="E155">
-        <f t="shared" si="27"/>
-        <v>32.299999999999997</v>
-      </c>
-      <c r="F155">
-        <f t="shared" si="28"/>
-        <v>15.299999999999999</v>
-      </c>
-      <c r="G155" t="e">
-        <f t="shared" si="29"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H155" t="e">
-        <f t="shared" si="30"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="162" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H162" s="52"/>
+    </row>
+    <row r="167" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D167" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>